<commit_message>
erro nas cores e nas formulas
</commit_message>
<xml_diff>
--- a/Previsao.xlsx
+++ b/Previsao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Desktop/Desktop_iCloud/Universidade/3ºano/2ºsemestre/MEIO/InventoryManagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D30B7A1-4FB3-6748-B22A-F5BAD0F17F69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DD8C90-8A83-3446-B2EE-A1063D906D61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0D2C59F3-1D13-48BD-903E-89ECABAE3337}"/>
   </bookViews>
@@ -526,82 +526,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002CE9F5-C0CF-6F4A-9226-C15012BC27ED}">
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -939,61 +939,61 @@
   <sheetData>
     <row r="2" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="25" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
-        <v>0</v>
-      </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37">
-        <f ca="1">INT(RAND()*419)</f>
-        <v>252</v>
-      </c>
-      <c r="G4" s="42"/>
+      <c r="A4" s="26">
+        <v>0</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29">
+        <f ca="1">INT(RANDBETWEEN(347,575))</f>
+        <v>366</v>
+      </c>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="35">
+      <c r="A5" s="27">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <f ca="1">F4</f>
-        <v>252</v>
+        <v>366</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="38">
-        <f ca="1">INT(_xlfn.NORM.INV(RAND(), 435.03, 37.85))</f>
-        <v>382</v>
+      <c r="E5" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>377</v>
       </c>
       <c r="F5" s="1">
         <f ca="1">B5-E5+D5</f>
-        <v>-130</v>
-      </c>
-      <c r="G5" s="43"/>
+        <v>-11</v>
+      </c>
+      <c r="G5" s="35"/>
       <c r="I5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1005,26 +1005,26 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="35">
+      <c r="A6" s="27">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B54" ca="1" si="0">F5</f>
-        <v>-130</v>
+        <v>-11</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="38">
-        <f t="shared" ref="E6:E20" ca="1" si="1">INT(_xlfn.NORM.INV(RAND(), 435.03, 37.85))</f>
-        <v>376</v>
+      <c r="E6" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>403</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F54" ca="1" si="2">B6-E6+D6</f>
-        <v>-506</v>
-      </c>
-      <c r="G6" s="43">
+        <f t="shared" ref="F6:F54" ca="1" si="1">B6-E6+D6</f>
+        <v>-414</v>
+      </c>
+      <c r="G6" s="35">
         <f ca="1">IF(F6 &lt; J29, (J28-F6), 0 )</f>
-        <v>1506</v>
+        <v>1414</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>7</v>
@@ -1037,30 +1037,30 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="35">
+      <c r="A7" s="27">
         <v>3</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-506</v>
+        <v>-414</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">IF(C7 = 0.6, G6, 0)</f>
-        <v>1506</v>
-      </c>
-      <c r="E7" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>468</v>
+        <v>0</v>
+      </c>
+      <c r="E7" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>471</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>532</v>
-      </c>
-      <c r="G7" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-885</v>
+      </c>
+      <c r="G7" s="35"/>
       <c r="I7" s="9" t="s">
         <v>8</v>
       </c>
@@ -1072,29 +1072,29 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
+      <c r="A8" s="27">
         <v>4</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>532</v>
+        <v>-885</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <f ca="1">IF(C7 = 0.4, G6, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>454</v>
+        <v>1414</v>
+      </c>
+      <c r="E8" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>398</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>78</v>
-      </c>
-      <c r="G8" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="G8" s="35">
         <f ca="1">IF(F8 &lt; J29, (J28-F8), 0 )</f>
-        <v>922</v>
+        <v>869</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>9</v>
@@ -1107,12 +1107,12 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
+      <c r="A9" s="27">
         <v>5</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="C9" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1120,42 +1120,42 @@
       </c>
       <c r="D9" s="1">
         <f ca="1">IF(C9 = 0.6, G8, 0)</f>
-        <v>922</v>
-      </c>
-      <c r="E9" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>425</v>
+        <v>869</v>
+      </c>
+      <c r="E9" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>399</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>575</v>
-      </c>
-      <c r="G9" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>601</v>
+      </c>
+      <c r="G9" s="35"/>
     </row>
     <row r="10" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="35">
+      <c r="A10" s="27">
         <v>6</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>575</v>
+        <v>601</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
         <f ca="1">IF(C9 = 0.4, G8, 0)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>401</v>
+      <c r="E10" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>370</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>174</v>
-      </c>
-      <c r="G10" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>231</v>
+      </c>
+      <c r="G10" s="35">
         <f ca="1">IF(F10 &lt; J29, (J28-F10), 0 )</f>
-        <v>826</v>
+        <v>769</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>11</v>
@@ -1165,12 +1165,12 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="35">
+      <c r="A11" s="27">
         <v>7</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>231</v>
       </c>
       <c r="C11" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1180,15 +1180,15 @@
         <f ca="1">IF(C11 = 0.6, G10, 0)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>421</v>
+      <c r="E11" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>423</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-247</v>
-      </c>
-      <c r="G11" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-192</v>
+      </c>
+      <c r="G11" s="35"/>
       <c r="I11" s="9">
         <v>1</v>
       </c>
@@ -1197,29 +1197,29 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
+      <c r="A12" s="27">
         <v>8</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-247</v>
+        <v>-192</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
         <f ca="1">IF(C11 = 0.4, G10, 0)</f>
-        <v>826</v>
-      </c>
-      <c r="E12" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>422</v>
+        <v>769</v>
+      </c>
+      <c r="E12" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>387</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>157</v>
-      </c>
-      <c r="G12" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="G12" s="35">
         <f ca="1">IF(F12 &lt; J29, (J28-F12), 0 )</f>
-        <v>843</v>
+        <v>810</v>
       </c>
       <c r="I12" s="11">
         <v>2</v>
@@ -1229,12 +1229,12 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="35">
+      <c r="A13" s="27">
         <v>9</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1242,114 +1242,114 @@
       </c>
       <c r="D13" s="1">
         <f ca="1">IF(C13 = 0.6, G12, 0)</f>
-        <v>843</v>
-      </c>
-      <c r="E13" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>469</v>
+        <v>810</v>
+      </c>
+      <c r="E13" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>405</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>531</v>
-      </c>
-      <c r="G13" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>595</v>
+      </c>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="35">
+      <c r="A14" s="27">
         <v>10</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>531</v>
+        <v>595</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <f ca="1">IF(C13 = 0.4, G12, 0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>413</v>
+      <c r="E14" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>412</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G14" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="G14" s="35">
         <f ca="1">IF(F14 &lt; J29, (J28-F14), 0 )</f>
-        <v>882</v>
+        <v>817</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35">
+      <c r="A15" s="27">
         <v>11</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>118</v>
+        <v>183</v>
       </c>
       <c r="C15" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D15" s="1">
         <f ca="1">IF(C15 = 0.6, G14, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>447</v>
+        <v>817</v>
+      </c>
+      <c r="E15" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>409</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-329</v>
-      </c>
-      <c r="G15" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>591</v>
+      </c>
+      <c r="G15" s="35"/>
       <c r="M15" s="15"/>
     </row>
     <row r="16" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
+      <c r="A16" s="27">
         <v>12</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-329</v>
+        <v>591</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <f ca="1">IF(C15 = 0.4, G14, 0)</f>
-        <v>882</v>
-      </c>
-      <c r="E16" s="38">
-        <f t="shared" ca="1" si="1"/>
-        <v>401</v>
+        <v>0</v>
+      </c>
+      <c r="E16" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>459</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>152</v>
-      </c>
-      <c r="G16" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="G16" s="35">
         <f ca="1">IF(F16 &lt; J29, (J28-F16), 0 )</f>
-        <v>848</v>
+        <v>868</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="21">
         <v>96.5</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="23"/>
+      <c r="L16" s="43"/>
     </row>
     <row r="17" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35">
+      <c r="A17" s="27">
         <v>13</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="C17" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1357,256 +1357,256 @@
       </c>
       <c r="D17" s="1">
         <f ca="1">IF(C17 = 0.6, G16, 0)</f>
-        <v>848</v>
-      </c>
-      <c r="E17" s="39">
-        <f t="shared" ca="1" si="1"/>
-        <v>471</v>
+        <v>868</v>
+      </c>
+      <c r="E17" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>421</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>529</v>
-      </c>
-      <c r="G17" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>579</v>
+      </c>
+      <c r="G17" s="35"/>
       <c r="I17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="21">
         <v>0.18</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="21"/>
+      <c r="L17" s="41"/>
     </row>
     <row r="18" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35">
+      <c r="A18" s="27">
         <v>14</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>529</v>
+        <v>579</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <f ca="1">IF(C17 = 0.4, G16, 0)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="39">
-        <f t="shared" ca="1" si="1"/>
-        <v>397</v>
+      <c r="E18" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>428</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>132</v>
-      </c>
-      <c r="G18" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>151</v>
+      </c>
+      <c r="G18" s="35">
         <f ca="1">IF(F18 &lt; J29, (J28-F18), 0 )</f>
-        <v>868</v>
+        <v>849</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="26">
+      <c r="J18" s="21">
         <f>J16*J17</f>
         <v>17.37</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="K18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="21"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35">
+      <c r="A19" s="27">
         <v>15</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="C19" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D19" s="1">
         <f ca="1">IF(C19 = 0.6, G18, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="39">
-        <f t="shared" ca="1" si="1"/>
-        <v>367</v>
+        <v>849</v>
+      </c>
+      <c r="E19" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>427</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-235</v>
-      </c>
-      <c r="G19" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>573</v>
+      </c>
+      <c r="G19" s="35"/>
     </row>
     <row r="20" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
+      <c r="A20" s="27">
         <v>16</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-235</v>
+        <v>573</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <f ca="1">IF(C19 = 0.4, G18, 0)</f>
-        <v>868</v>
-      </c>
-      <c r="E20" s="39">
-        <f t="shared" ca="1" si="1"/>
-        <v>365</v>
+        <v>0</v>
+      </c>
+      <c r="E20" s="30">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
+        <v>398</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>268</v>
-      </c>
-      <c r="G20" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>175</v>
+      </c>
+      <c r="G20" s="35">
         <f ca="1">IF(F20 &lt; J29, (J28-F20), 0 )</f>
-        <v>732</v>
+        <v>825</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20" s="21">
         <v>7</v>
       </c>
-      <c r="K20" s="24" t="s">
+      <c r="K20" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="20"/>
+      <c r="L20" s="18"/>
       <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35">
+      <c r="A21" s="27">
         <v>17</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>268</v>
+        <v>175</v>
       </c>
       <c r="C21" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D21" s="1">
         <f ca="1">IF(C21 = 0.6, G20, 0)</f>
-        <v>732</v>
-      </c>
-      <c r="E21" s="39">
-        <f ca="1">INT(_xlfn.NORM.INV(RAND(), 575.26, 50.05))</f>
-        <v>638</v>
+        <v>0</v>
+      </c>
+      <c r="E21" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>576</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>362</v>
-      </c>
-      <c r="G21" s="43"/>
-      <c r="I21" s="25" t="s">
+        <f t="shared" ca="1" si="1"/>
+        <v>-401</v>
+      </c>
+      <c r="G21" s="35"/>
+      <c r="I21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="21">
         <f>20+2*J20</f>
         <v>34</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="18"/>
+      <c r="L21" s="38"/>
     </row>
     <row r="22" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
+      <c r="A22" s="27">
         <v>18</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>362</v>
+        <v>-401</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <f ca="1">IF(C21 = 0.4, G20, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="39">
-        <f t="shared" ref="E22:E32" ca="1" si="3">INT(_xlfn.NORM.INV(RAND(), 575.26, 50.05))</f>
-        <v>637</v>
+        <v>825</v>
+      </c>
+      <c r="E22" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>576</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-275</v>
-      </c>
-      <c r="G22" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-152</v>
+      </c>
+      <c r="G22" s="35">
         <f ca="1">IF(F22 &lt; J29, (J28-F22), 0 )</f>
-        <v>1275</v>
+        <v>1152</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
     </row>
     <row r="23" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35">
+      <c r="A23" s="27">
         <v>19</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-275</v>
+        <v>-152</v>
       </c>
       <c r="C23" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D23" s="1">
         <f ca="1">IF(C23 = 0.6, G22, 0)</f>
-        <v>1275</v>
-      </c>
-      <c r="E23" s="39">
-        <f t="shared" ca="1" si="3"/>
-        <v>602</v>
+        <v>0</v>
+      </c>
+      <c r="E23" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>597</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>398</v>
-      </c>
-      <c r="G23" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-749</v>
+      </c>
+      <c r="G23" s="35"/>
       <c r="I23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="26">
+      <c r="J23" s="21">
         <v>900</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="L23" s="18"/>
+      <c r="L23" s="38"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35">
+      <c r="A24" s="27">
         <v>20</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>398</v>
+        <v>-749</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <f ca="1">IF(C23 = 0.4, G22, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="39">
-        <f t="shared" ca="1" si="3"/>
-        <v>576</v>
+        <v>1152</v>
+      </c>
+      <c r="E24" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>620</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-178</v>
-      </c>
-      <c r="G24" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-217</v>
+      </c>
+      <c r="G24" s="35">
         <f ca="1">IF(F24 &lt; J29, (J28-F24), 0 )</f>
-        <v>1178</v>
+        <v>1217</v>
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -1614,12 +1614,12 @@
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35">
+      <c r="A25" s="27">
         <v>21</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-178</v>
+        <v>-217</v>
       </c>
       <c r="C25" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1629,121 +1629,121 @@
         <f ca="1">IF(C25 = 0.6, G24, 0)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="39">
-        <f t="shared" ca="1" si="3"/>
-        <v>567</v>
+      <c r="E25" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>592</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-745</v>
-      </c>
-      <c r="G25" s="43"/>
-      <c r="I25" s="25" t="s">
+        <f t="shared" ca="1" si="1"/>
+        <v>-809</v>
+      </c>
+      <c r="G25" s="35"/>
+      <c r="I25" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="26">
+      <c r="J25" s="21">
         <v>2</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="18"/>
+      <c r="L25" s="38"/>
     </row>
     <row r="26" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35">
+      <c r="A26" s="27">
         <v>22</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-745</v>
+        <v>-809</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
         <f ca="1">IF(C25 = 0.4, G24, 0)</f>
-        <v>1178</v>
-      </c>
-      <c r="E26" s="39">
-        <f t="shared" ca="1" si="3"/>
-        <v>440</v>
+        <v>1217</v>
+      </c>
+      <c r="E26" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>646</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-7</v>
-      </c>
-      <c r="G26" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-238</v>
+      </c>
+      <c r="G26" s="35">
         <f ca="1">IF(F26 &lt; J29, (J28-F26), 0 )</f>
-        <v>1007</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A27" s="35">
+      <c r="A27" s="27">
         <v>23</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-238</v>
       </c>
       <c r="C27" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D27" s="1">
         <f ca="1">IF(C27 = 0.6, G26, 0)</f>
-        <v>1007</v>
-      </c>
-      <c r="E27" s="39">
-        <f t="shared" ca="1" si="3"/>
-        <v>543</v>
+        <v>0</v>
+      </c>
+      <c r="E27" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>622</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>457</v>
-      </c>
-      <c r="G27" s="43"/>
-      <c r="I27" s="28" t="s">
+        <f t="shared" ca="1" si="1"/>
+        <v>-860</v>
+      </c>
+      <c r="G27" s="35"/>
+      <c r="I27" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="29"/>
+      <c r="J27" s="40"/>
     </row>
     <row r="28" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A28" s="35">
+      <c r="A28" s="27">
         <v>24</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>457</v>
+        <v>-860</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
         <f ca="1">IF(C27 = 0.4, G26, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="39">
-        <f t="shared" ca="1" si="3"/>
-        <v>529</v>
+        <v>1238</v>
+      </c>
+      <c r="E28" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>592</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-72</v>
-      </c>
-      <c r="G28" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-214</v>
+      </c>
+      <c r="G28" s="35">
         <f ca="1">IF(F28 &lt; J29, (J28-F28), 0 )</f>
-        <v>1072</v>
+        <v>1214</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="30">
+      <c r="J28" s="22">
         <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35">
+      <c r="A29" s="27">
         <v>25</v>
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-72</v>
+        <v>-214</v>
       </c>
       <c r="C29" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1753,159 +1753,159 @@
         <f ca="1">IF(C29 = 0.6, G28, 0)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="40">
-        <f t="shared" ca="1" si="3"/>
-        <v>544</v>
+      <c r="E29" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>603</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-616</v>
-      </c>
-      <c r="G29" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-817</v>
+      </c>
+      <c r="G29" s="35"/>
       <c r="I29" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="31">
-        <v>500</v>
+      <c r="J29" s="23">
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A30" s="35">
+      <c r="A30" s="27">
         <v>26</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-616</v>
+        <v>-817</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <f ca="1">IF(C29 = 0.4, G28, 0)</f>
-        <v>1072</v>
-      </c>
-      <c r="E30" s="40">
-        <f t="shared" ca="1" si="3"/>
-        <v>519</v>
+        <v>1214</v>
+      </c>
+      <c r="E30" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>592</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-63</v>
-      </c>
-      <c r="G30" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-195</v>
+      </c>
+      <c r="G30" s="35">
         <f ca="1">IF(F30 &lt; J29, (J28-F30), 0 )</f>
-        <v>1063</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" s="35">
+      <c r="A31" s="27">
         <v>27</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-63</v>
+        <v>-195</v>
       </c>
       <c r="C31" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D31" s="1">
         <f ca="1">IF(C31 = 0.6, G30, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="40">
-        <f t="shared" ca="1" si="3"/>
-        <v>634</v>
+        <v>1195</v>
+      </c>
+      <c r="E31" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>531</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-697</v>
-      </c>
-      <c r="G31" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>469</v>
+      </c>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A32" s="35">
+      <c r="A32" s="27">
         <v>28</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-697</v>
+        <v>469</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
         <f ca="1">IF(C31 = 0.4, G30, 0)</f>
-        <v>1063</v>
-      </c>
-      <c r="E32" s="40">
-        <f t="shared" ca="1" si="3"/>
-        <v>613</v>
+        <v>0</v>
+      </c>
+      <c r="E32" s="31">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
+        <v>547</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-247</v>
-      </c>
-      <c r="G32" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-78</v>
+      </c>
+      <c r="G32" s="35">
         <f ca="1">IF(F32 &lt; J29, (J28-F32), 0 )</f>
-        <v>1247</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A33" s="35">
+      <c r="A33" s="27">
         <v>29</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-247</v>
+        <v>-78</v>
       </c>
       <c r="C33" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D33" s="1">
         <f ca="1">IF(C33 = 0.6, G32, 0)</f>
-        <v>1247</v>
-      </c>
-      <c r="E33" s="40">
-        <f ca="1">INT(_xlfn.NORM.INV(RAND(), 347.31, 30.22))</f>
-        <v>408</v>
+        <v>0</v>
+      </c>
+      <c r="E33" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>339</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>592</v>
-      </c>
-      <c r="G33" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-417</v>
+      </c>
+      <c r="G33" s="35"/>
     </row>
     <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A34" s="35">
+      <c r="A34" s="27">
         <v>30</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>592</v>
+        <v>-417</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
         <f ca="1">IF(C33 = 0.4, G32, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="40">
-        <f t="shared" ref="E34:E54" ca="1" si="4">INT(_xlfn.NORM.INV(RAND(), 347.31, 30.22))</f>
-        <v>321</v>
+        <v>1078</v>
+      </c>
+      <c r="E34" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>335</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>271</v>
-      </c>
-      <c r="G34" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>326</v>
+      </c>
+      <c r="G34" s="35">
         <f ca="1">IF(F34 &lt; J29, (J28-F34), 0 )</f>
-        <v>729</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A35" s="35">
+      <c r="A35" s="27">
         <v>31</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>271</v>
+        <v>326</v>
       </c>
       <c r="C35" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1913,259 +1913,259 @@
       </c>
       <c r="D35" s="1">
         <f ca="1">IF(C35 = 0.6, G34, 0)</f>
-        <v>729</v>
-      </c>
-      <c r="E35" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>344</v>
+        <v>0</v>
+      </c>
+      <c r="E35" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>340</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>656</v>
-      </c>
-      <c r="G35" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-14</v>
+      </c>
+      <c r="G35" s="35"/>
     </row>
     <row r="36" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A36" s="35">
+      <c r="A36" s="27">
         <v>32</v>
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>656</v>
+        <v>-14</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
         <f ca="1">IF(C35 = 0.4, G34, 0)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>350</v>
+      <c r="E36" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>285</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>306</v>
-      </c>
-      <c r="G36" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-299</v>
+      </c>
+      <c r="G36" s="35">
         <f ca="1">IF(F36 &lt; J29, (J28-F36), 0 )</f>
-        <v>694</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A37" s="35">
+      <c r="A37" s="27">
         <v>33</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>306</v>
+        <v>-299</v>
       </c>
       <c r="C37" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D37" s="1">
         <f ca="1">IF(C37 = 0.6, G36, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>322</v>
+        <v>1299</v>
+      </c>
+      <c r="E37" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>369</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-16</v>
-      </c>
-      <c r="G37" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>631</v>
+      </c>
+      <c r="G37" s="35"/>
     </row>
     <row r="38" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A38" s="35">
+      <c r="A38" s="27">
         <v>34</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-16</v>
+        <v>631</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
         <f ca="1">IF(C37 = 0.4, G36, 0)</f>
-        <v>694</v>
-      </c>
-      <c r="E38" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>324</v>
+        <v>0</v>
+      </c>
+      <c r="E38" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>350</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>354</v>
-      </c>
-      <c r="G38" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>281</v>
+      </c>
+      <c r="G38" s="35">
         <f ca="1">IF(F38 &lt; J29, (J28-F38), 0 )</f>
-        <v>646</v>
+        <v>719</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A39" s="35">
+      <c r="A39" s="27">
         <v>35</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>354</v>
+        <v>281</v>
       </c>
       <c r="C39" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D39" s="1">
         <f ca="1">IF(C39 = 0.6, G38, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>370</v>
+        <v>719</v>
+      </c>
+      <c r="E39" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>324</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-16</v>
-      </c>
-      <c r="G39" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>676</v>
+      </c>
+      <c r="G39" s="35"/>
     </row>
     <row r="40" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A40" s="35">
+      <c r="A40" s="27">
         <v>36</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-16</v>
+        <v>676</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1">
         <f ca="1">IF(C39 = 0.4, G38, 0)</f>
-        <v>646</v>
-      </c>
-      <c r="E40" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>323</v>
+        <v>0</v>
+      </c>
+      <c r="E40" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>381</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>307</v>
-      </c>
-      <c r="G40" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>295</v>
+      </c>
+      <c r="G40" s="35">
         <f ca="1">IF(F40 &lt; J29, (J28-F40), 0 )</f>
-        <v>693</v>
+        <v>705</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A41" s="35">
+      <c r="A41" s="27">
         <v>37</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="C41" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D41" s="1">
         <f ca="1">IF(C41 = 0.6, G40, 0)</f>
-        <v>693</v>
-      </c>
-      <c r="E41" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>396</v>
+        <v>0</v>
+      </c>
+      <c r="E41" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>322</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>604</v>
-      </c>
-      <c r="G41" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-27</v>
+      </c>
+      <c r="G41" s="35"/>
     </row>
     <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A42" s="35">
+      <c r="A42" s="27">
         <v>38</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>604</v>
+        <v>-27</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1">
         <f ca="1">IF(C41 = 0.4, G40, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>332</v>
+        <v>705</v>
+      </c>
+      <c r="E42" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>259</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>272</v>
-      </c>
-      <c r="G42" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>419</v>
+      </c>
+      <c r="G42" s="35">
         <f ca="1">IF(F42 &lt; J29, (J28-F42), 0 )</f>
-        <v>728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A43" s="35">
+      <c r="A43" s="27">
         <v>39</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>272</v>
+        <v>419</v>
       </c>
       <c r="C43" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D43" s="1">
         <f ca="1">IF(C43 = 0.6, G42, 0)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>358</v>
+      <c r="E43" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>409</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-86</v>
-      </c>
-      <c r="G43" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G43" s="35"/>
     </row>
     <row r="44" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A44" s="35">
+      <c r="A44" s="27">
         <v>40</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-86</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1">
         <f ca="1">IF(C43 = 0.4, G42, 0)</f>
-        <v>728</v>
-      </c>
-      <c r="E44" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>366</v>
+        <v>0</v>
+      </c>
+      <c r="E44" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>304</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>276</v>
-      </c>
-      <c r="G44" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-294</v>
+      </c>
+      <c r="G44" s="35">
         <f ca="1">IF(F44 &lt; J29, (J28-F44), 0 )</f>
-        <v>724</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A45" s="35">
+      <c r="A45" s="27">
         <v>41</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>276</v>
+        <v>-294</v>
       </c>
       <c r="C45" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2175,49 +2175,49 @@
         <f ca="1">IF(C45 = 0.6, G44, 0)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>387</v>
+      <c r="E45" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>296</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-111</v>
-      </c>
-      <c r="G45" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-590</v>
+      </c>
+      <c r="G45" s="35"/>
     </row>
     <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A46" s="35">
+      <c r="A46" s="27">
         <v>42</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-111</v>
+        <v>-590</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1">
         <f ca="1">IF(C45 = 0.4, G44, 0)</f>
-        <v>724</v>
-      </c>
-      <c r="E46" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>350</v>
+        <v>1294</v>
+      </c>
+      <c r="E46" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>311</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>263</v>
-      </c>
-      <c r="G46" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>393</v>
+      </c>
+      <c r="G46" s="35">
         <f ca="1">IF(F46 &lt; J29, (J28-F46), 0 )</f>
-        <v>737</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A47" s="35">
+      <c r="A47" s="27">
         <v>43</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>263</v>
+        <v>393</v>
       </c>
       <c r="C47" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2225,51 +2225,51 @@
       </c>
       <c r="D47" s="1">
         <f ca="1">IF(C47 = 0.6, G46, 0)</f>
-        <v>737</v>
-      </c>
-      <c r="E47" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>360</v>
+        <v>0</v>
+      </c>
+      <c r="E47" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>307</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>640</v>
-      </c>
-      <c r="G47" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="G47" s="35"/>
     </row>
     <row r="48" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A48" s="35">
+      <c r="A48" s="27">
         <v>44</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>640</v>
+        <v>86</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
         <f ca="1">IF(C47 = 0.4, G46, 0)</f>
         <v>0</v>
       </c>
-      <c r="E48" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>319</v>
+      <c r="E48" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>345</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>321</v>
-      </c>
-      <c r="G48" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-259</v>
+      </c>
+      <c r="G48" s="35">
         <f ca="1">IF(F48 &lt; J29, (J28-F48), 0 )</f>
-        <v>679</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A49" s="35">
+      <c r="A49" s="27">
         <v>45</v>
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>321</v>
+        <v>-259</v>
       </c>
       <c r="C49" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2279,49 +2279,49 @@
         <f ca="1">IF(C49 = 0.6, G48, 0)</f>
         <v>0</v>
       </c>
-      <c r="E49" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>336</v>
+      <c r="E49" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>319</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>-15</v>
-      </c>
-      <c r="G49" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-578</v>
+      </c>
+      <c r="G49" s="35"/>
     </row>
     <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A50" s="35">
+      <c r="A50" s="27">
         <v>46</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-15</v>
+        <v>-578</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1">
         <f ca="1">IF(C49 = 0.4, G48, 0)</f>
-        <v>679</v>
-      </c>
-      <c r="E50" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>326</v>
+        <v>1259</v>
+      </c>
+      <c r="E50" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>402</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>338</v>
-      </c>
-      <c r="G50" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>279</v>
+      </c>
+      <c r="G50" s="35">
         <f ca="1">IF(F50 &lt; J29, (J28-F50), 0 )</f>
-        <v>662</v>
+        <v>721</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A51" s="35">
+      <c r="A51" s="27">
         <v>47</v>
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>338</v>
+        <v>279</v>
       </c>
       <c r="C51" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2331,49 +2331,49 @@
         <f ca="1">IF(C51 = 0.6, G50, 0)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>317</v>
+      <c r="E51" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>342</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="G51" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-63</v>
+      </c>
+      <c r="G51" s="35"/>
     </row>
     <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A52" s="35">
+      <c r="A52" s="27">
         <v>48</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>-63</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1">
         <f ca="1">IF(C51 = 0.4, G50, 0)</f>
-        <v>662</v>
-      </c>
-      <c r="E52" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>327</v>
+        <v>721</v>
+      </c>
+      <c r="E52" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>342</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>356</v>
-      </c>
-      <c r="G52" s="43">
+        <f t="shared" ca="1" si="1"/>
+        <v>316</v>
+      </c>
+      <c r="G52" s="35">
         <f ca="1">IF(F52 &lt; J29, (J28-F52), 0 )</f>
-        <v>644</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A53" s="35">
+      <c r="A53" s="27">
         <v>49</v>
       </c>
       <c r="B53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>356</v>
+        <v>316</v>
       </c>
       <c r="C53" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2383,52 +2383,52 @@
         <f ca="1">IF(C53 = 0.6, G52, 0)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="40">
-        <f t="shared" ca="1" si="4"/>
-        <v>322</v>
+      <c r="E53" s="32">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>328</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="G53" s="43"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>-12</v>
+      </c>
+      <c r="G53" s="35"/>
     </row>
     <row r="54" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="36">
+      <c r="A54" s="28">
         <v>50</v>
       </c>
       <c r="B54" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>-12</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
         <f ca="1">IF(C53 = 0.4, G52, 0)</f>
-        <v>644</v>
-      </c>
-      <c r="E54" s="41">
-        <f t="shared" ca="1" si="4"/>
-        <v>334</v>
+        <v>0</v>
+      </c>
+      <c r="E54" s="33">
+        <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
+        <v>354</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>344</v>
-      </c>
-      <c r="G54" s="44">
+        <f t="shared" ca="1" si="1"/>
+        <v>-366</v>
+      </c>
+      <c r="G54" s="36">
         <f ca="1">IF(F54 &lt; J29, (J28-F54), 0 )</f>
-        <v>656</v>
+        <v>1366</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
caso de quebra de inventario
</commit_message>
<xml_diff>
--- a/Previsao.xlsx
+++ b/Previsao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Desktop/Desktop_iCloud/Universidade/3ºano/2ºsemestre/MEIO/InventoryManagement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogobraga/Desktop/InventoryManagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DD8C90-8A83-3446-B2EE-A1063D906D61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FB9CFB-AA39-F74F-94BA-1C274D26010F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0D2C59F3-1D13-48BD-903E-89ECABAE3337}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{0D2C59F3-1D13-48BD-903E-89ECABAE3337}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulador" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>PERÍODO</t>
   </si>
@@ -127,6 +126,12 @@
   </si>
   <si>
     <t>STOCK EM MÃO (SM)</t>
+  </si>
+  <si>
+    <t>PERDA DE VENDAS</t>
+  </si>
+  <si>
+    <t>CASO DE QUEBRA DE INVENTARIO</t>
   </si>
 </sst>
 </file>
@@ -213,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -473,11 +478,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,6 +613,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -591,17 +636,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002CE9F5-C0CF-6F4A-9226-C15012BC27ED}">
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -932,8 +971,8 @@
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -971,7 +1010,7 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29">
         <f ca="1">INT(RANDBETWEEN(347,575))</f>
-        <v>366</v>
+        <v>528</v>
       </c>
       <c r="G4" s="34"/>
     </row>
@@ -981,17 +1020,17 @@
       </c>
       <c r="B5" s="1">
         <f ca="1">F4</f>
-        <v>366</v>
+        <v>528</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>377</v>
+        <v>398</v>
       </c>
       <c r="F5" s="1">
         <f ca="1">B5-E5+D5</f>
-        <v>-11</v>
+        <v>130</v>
       </c>
       <c r="G5" s="35"/>
       <c r="I5" s="6" t="s">
@@ -1010,21 +1049,21 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B54" ca="1" si="0">F5</f>
-        <v>-11</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>403</v>
+        <v>445</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6:F54" ca="1" si="1">B6-E6+D6</f>
-        <v>-414</v>
+        <v>-315</v>
       </c>
       <c r="G6" s="35">
-        <f ca="1">IF(F6 &lt; J29, (J28-F6), 0 )</f>
-        <v>1414</v>
+        <f ca="1">IF(F6 &lt; J29, (IF(F6&lt;0, J28, J28-F6)), 0 )</f>
+        <v>1000</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>7</v>
@@ -1042,23 +1081,23 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-414</v>
+        <v>-315</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">IF(C7 = 0.6, G6, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E7" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>471</v>
+        <v>348</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-885</v>
+        <v>337</v>
       </c>
       <c r="G7" s="35"/>
       <c r="I7" s="9" t="s">
@@ -1077,24 +1116,24 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-885</v>
+        <v>337</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <f ca="1">IF(C7 = 0.4, G6, 0)</f>
-        <v>1414</v>
+        <v>0</v>
       </c>
       <c r="E8" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>398</v>
+        <v>465</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>131</v>
+        <v>-128</v>
       </c>
       <c r="G8" s="35">
-        <f ca="1">IF(F8 &lt; J29, (J28-F8), 0 )</f>
-        <v>869</v>
+        <f ca="1">IF(F8 &lt; J29, (IF(F8&lt;0, J28, J28-F8)), 0 )</f>
+        <v>1000</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>9</v>
@@ -1112,7 +1151,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>131</v>
+        <v>-128</v>
       </c>
       <c r="C9" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1120,15 +1159,15 @@
       </c>
       <c r="D9" s="1">
         <f ca="1">IF(C9 = 0.6, G8, 0)</f>
-        <v>869</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>601</v>
+        <v>482</v>
       </c>
       <c r="G9" s="35"/>
     </row>
@@ -1138,7 +1177,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>601</v>
+        <v>482</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
@@ -1147,15 +1186,15 @@
       </c>
       <c r="E10" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>370</v>
+        <v>445</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>231</v>
+        <v>37</v>
       </c>
       <c r="G10" s="35">
-        <f ca="1">IF(F10 &lt; J29, (J28-F10), 0 )</f>
-        <v>769</v>
+        <f ca="1">IF(F10 &lt; J29, (IF(F10&lt;0, J28, J28-F10)), 0 )</f>
+        <v>963</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>11</v>
@@ -1170,7 +1209,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>231</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1182,11 +1221,11 @@
       </c>
       <c r="E11" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>423</v>
+        <v>385</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-192</v>
+        <v>-348</v>
       </c>
       <c r="G11" s="35"/>
       <c r="I11" s="9">
@@ -1202,24 +1241,24 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-192</v>
+        <v>-348</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
         <f ca="1">IF(C11 = 0.4, G10, 0)</f>
-        <v>769</v>
+        <v>963</v>
       </c>
       <c r="E12" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>387</v>
+        <v>461</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="G12" s="35">
-        <f ca="1">IF(F12 &lt; J29, (J28-F12), 0 )</f>
-        <v>810</v>
+        <f ca="1">IF(F12 &lt; J29, (IF(F12&lt;0, J28, J28-F12)), 0 )</f>
+        <v>846</v>
       </c>
       <c r="I12" s="11">
         <v>2</v>
@@ -1234,7 +1273,7 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1242,15 +1281,15 @@
       </c>
       <c r="D13" s="1">
         <f ca="1">IF(C13 = 0.6, G12, 0)</f>
-        <v>810</v>
+        <v>846</v>
       </c>
       <c r="E13" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G13" s="35"/>
     </row>
@@ -1260,7 +1299,7 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
@@ -1269,15 +1308,15 @@
       </c>
       <c r="E14" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>412</v>
+        <v>382</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="G14" s="35">
-        <f ca="1">IF(F14 &lt; J29, (J28-F14), 0 )</f>
-        <v>817</v>
+        <f ca="1">IF(F14 &lt; J29, (IF(F14&lt;0, J28, J28-F14)), 0 )</f>
+        <v>788</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -1286,7 +1325,7 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="C15" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1294,15 +1333,15 @@
       </c>
       <c r="D15" s="1">
         <f ca="1">IF(C15 = 0.6, G14, 0)</f>
-        <v>817</v>
+        <v>788</v>
       </c>
       <c r="E15" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>409</v>
+        <v>478</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>591</v>
+        <v>522</v>
       </c>
       <c r="G15" s="35"/>
       <c r="M15" s="15"/>
@@ -1313,7 +1352,7 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>591</v>
+        <v>522</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
@@ -1322,15 +1361,15 @@
       </c>
       <c r="E16" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="G16" s="35">
-        <f ca="1">IF(F16 &lt; J29, (J28-F16), 0 )</f>
-        <v>868</v>
+        <f ca="1">IF(F16 &lt; J29, (IF(F16&lt;0, J28, J28-F16)), 0 )</f>
+        <v>928</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>15</v>
@@ -1338,10 +1377,10 @@
       <c r="J16" s="21">
         <v>96.5</v>
       </c>
-      <c r="K16" s="42" t="s">
+      <c r="K16" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="43"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
@@ -1349,7 +1388,7 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1357,15 +1396,15 @@
       </c>
       <c r="D17" s="1">
         <f ca="1">IF(C17 = 0.6, G16, 0)</f>
-        <v>868</v>
+        <v>928</v>
       </c>
       <c r="E17" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>421</v>
+        <v>354</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>579</v>
+        <v>646</v>
       </c>
       <c r="G17" s="35"/>
       <c r="I17" s="17" t="s">
@@ -1374,10 +1413,10 @@
       <c r="J17" s="21">
         <v>0.18</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="41"/>
+      <c r="L17" s="39"/>
     </row>
     <row r="18" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
@@ -1385,7 +1424,7 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>579</v>
+        <v>646</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
@@ -1394,15 +1433,15 @@
       </c>
       <c r="E18" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>151</v>
+        <v>221</v>
       </c>
       <c r="G18" s="35">
-        <f ca="1">IF(F18 &lt; J29, (J28-F18), 0 )</f>
-        <v>849</v>
+        <f ca="1">IF(F18 &lt; J29, (IF(F18&lt;0, J28, J28-F18)), 0 )</f>
+        <v>779</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>19</v>
@@ -1411,10 +1450,10 @@
         <f>J16*J17</f>
         <v>17.37</v>
       </c>
-      <c r="K18" s="42" t="s">
+      <c r="K18" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="41"/>
+      <c r="L18" s="39"/>
     </row>
     <row r="19" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
@@ -1422,7 +1461,7 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>151</v>
+        <v>221</v>
       </c>
       <c r="C19" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1430,15 +1469,15 @@
       </c>
       <c r="D19" s="1">
         <f ca="1">IF(C19 = 0.6, G18, 0)</f>
-        <v>849</v>
+        <v>779</v>
       </c>
       <c r="E19" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>427</v>
+        <v>442</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>573</v>
+        <v>558</v>
       </c>
       <c r="G19" s="35"/>
     </row>
@@ -1448,7 +1487,7 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>573</v>
+        <v>558</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
@@ -1457,15 +1496,15 @@
       </c>
       <c r="E20" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>398</v>
+        <v>370</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="G20" s="35">
-        <f ca="1">IF(F20 &lt; J29, (J28-F20), 0 )</f>
-        <v>825</v>
+        <f ca="1">IF(F20 &lt; J29, (IF(F20&lt;0, J28, J28-F20)), 0 )</f>
+        <v>812</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>13</v>
@@ -1485,23 +1524,23 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="C21" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D21" s="1">
         <f ca="1">IF(C21 = 0.6, G20, 0)</f>
-        <v>0</v>
+        <v>812</v>
       </c>
       <c r="E21" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>576</v>
+        <v>592</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-401</v>
+        <v>408</v>
       </c>
       <c r="G21" s="35"/>
       <c r="I21" s="20" t="s">
@@ -1511,10 +1550,10 @@
         <f>20+2*J20</f>
         <v>34</v>
       </c>
-      <c r="K21" s="37" t="s">
+      <c r="K21" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="38"/>
+      <c r="L21" s="42"/>
     </row>
     <row r="22" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
@@ -1522,29 +1561,29 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-401</v>
+        <v>408</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <f ca="1">IF(C21 = 0.4, G20, 0)</f>
-        <v>825</v>
+        <v>0</v>
       </c>
       <c r="E22" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>576</v>
+        <v>536</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-152</v>
+        <v>-128</v>
       </c>
       <c r="G22" s="35">
-        <f ca="1">IF(F22 &lt; J29, (J28-F22), 0 )</f>
-        <v>1152</v>
+        <f ca="1">IF(F22 &lt; J29, (IF(F22&lt;0, J28, J28-F22)), 0 )</f>
+        <v>1000</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
     </row>
     <row r="23" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
@@ -1552,7 +1591,7 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-152</v>
+        <v>-128</v>
       </c>
       <c r="C23" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1564,11 +1603,11 @@
       </c>
       <c r="E23" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>597</v>
+        <v>571</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-749</v>
+        <v>-699</v>
       </c>
       <c r="G23" s="35"/>
       <c r="I23" s="17" t="s">
@@ -1577,10 +1616,10 @@
       <c r="J23" s="21">
         <v>900</v>
       </c>
-      <c r="K23" s="37" t="s">
+      <c r="K23" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="L23" s="38"/>
+      <c r="L23" s="42"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -1589,24 +1628,24 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-749</v>
+        <v>-699</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <f ca="1">IF(C23 = 0.4, G22, 0)</f>
-        <v>1152</v>
+        <v>1000</v>
       </c>
       <c r="E24" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>620</v>
+        <v>558</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-217</v>
+        <v>-257</v>
       </c>
       <c r="G24" s="35">
-        <f ca="1">IF(F24 &lt; J29, (J28-F24), 0 )</f>
-        <v>1217</v>
+        <f ca="1">IF(F24 &lt; J29, (IF(F24&lt;0, J28, J28-F24)), 0 )</f>
+        <v>1000</v>
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -1619,23 +1658,23 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-217</v>
+        <v>-257</v>
       </c>
       <c r="C25" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D25" s="1">
         <f ca="1">IF(C25 = 0.6, G24, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E25" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-809</v>
+        <v>152</v>
       </c>
       <c r="G25" s="35"/>
       <c r="I25" s="20" t="s">
@@ -1644,10 +1683,10 @@
       <c r="J25" s="21">
         <v>2</v>
       </c>
-      <c r="K25" s="37" t="s">
+      <c r="K25" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="38"/>
+      <c r="L25" s="42"/>
     </row>
     <row r="26" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
@@ -1655,24 +1694,24 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-809</v>
+        <v>152</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
         <f ca="1">IF(C25 = 0.4, G24, 0)</f>
-        <v>1217</v>
+        <v>0</v>
       </c>
       <c r="E26" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>646</v>
+        <v>571</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-238</v>
+        <v>-419</v>
       </c>
       <c r="G26" s="35">
-        <f ca="1">IF(F26 &lt; J29, (J28-F26), 0 )</f>
-        <v>1238</v>
+        <f ca="1">IF(F26 &lt; J29, (IF(F26&lt;0, J28, J28-F26)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="19" x14ac:dyDescent="0.2">
@@ -1681,7 +1720,7 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-238</v>
+        <v>-419</v>
       </c>
       <c r="C27" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1693,17 +1732,17 @@
       </c>
       <c r="E27" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>622</v>
+        <v>527</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-860</v>
+        <v>-946</v>
       </c>
       <c r="G27" s="35"/>
-      <c r="I27" s="39" t="s">
+      <c r="I27" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="40"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:13" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
@@ -1711,24 +1750,24 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-860</v>
+        <v>-946</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
         <f ca="1">IF(C27 = 0.4, G26, 0)</f>
-        <v>1238</v>
+        <v>1000</v>
       </c>
       <c r="E28" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>592</v>
+        <v>556</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-214</v>
+        <v>-502</v>
       </c>
       <c r="G28" s="35">
-        <f ca="1">IF(F28 &lt; J29, (J28-F28), 0 )</f>
-        <v>1214</v>
+        <f ca="1">IF(F28 &lt; J29, (IF(F28&lt;0, J28, J28-F28)), 0 )</f>
+        <v>1000</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>28</v>
@@ -1743,7 +1782,7 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-214</v>
+        <v>-502</v>
       </c>
       <c r="C29" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1755,11 +1794,11 @@
       </c>
       <c r="E29" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>603</v>
+        <v>540</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-817</v>
+        <v>-1042</v>
       </c>
       <c r="G29" s="35"/>
       <c r="I29" s="11" t="s">
@@ -1769,39 +1808,39 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
         <v>26</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-817</v>
+        <v>-1042</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <f ca="1">IF(C29 = 0.4, G28, 0)</f>
-        <v>1214</v>
+        <v>1000</v>
       </c>
       <c r="E30" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>592</v>
+        <v>540</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-195</v>
+        <v>-582</v>
       </c>
       <c r="G30" s="35">
-        <f ca="1">IF(F30 &lt; J29, (J28-F30), 0 )</f>
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+        <f ca="1">IF(F30 &lt; J29, (IF(F30&lt;0, J28, J28-F30)), 0 )</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <v>27</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-195</v>
+        <v>-582</v>
       </c>
       <c r="C31" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1809,17 +1848,23 @@
       </c>
       <c r="D31" s="1">
         <f ca="1">IF(C31 = 0.6, G30, 0)</f>
-        <v>1195</v>
+        <v>1000</v>
       </c>
       <c r="E31" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>531</v>
+        <v>622</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>469</v>
+        <v>-204</v>
       </c>
       <c r="G31" s="35"/>
+      <c r="I31" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="46" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
@@ -1827,7 +1872,7 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>469</v>
+        <v>-204</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
@@ -1836,15 +1881,15 @@
       </c>
       <c r="E32" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-78</v>
+        <v>-744</v>
       </c>
       <c r="G32" s="35">
-        <f ca="1">IF(F32 &lt; J29, (J28-F32), 0 )</f>
-        <v>1078</v>
+        <f ca="1">IF(F32 &lt; J29, (IF(F32&lt;0, J28, J28-F32)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -1853,23 +1898,23 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-78</v>
+        <v>-744</v>
       </c>
       <c r="C33" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D33" s="1">
         <f ca="1">IF(C33 = 0.6, G32, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E33" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>339</v>
+        <v>371</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-417</v>
+        <v>-115</v>
       </c>
       <c r="G33" s="35"/>
     </row>
@@ -1879,24 +1924,24 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-417</v>
+        <v>-115</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
         <f ca="1">IF(C33 = 0.4, G32, 0)</f>
-        <v>1078</v>
+        <v>0</v>
       </c>
       <c r="E34" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>326</v>
+        <v>-471</v>
       </c>
       <c r="G34" s="35">
-        <f ca="1">IF(F34 &lt; J29, (J28-F34), 0 )</f>
-        <v>0</v>
+        <f ca="1">IF(F34 &lt; J29, (IF(F34&lt;0, J28, J28-F34)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -1905,7 +1950,7 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>326</v>
+        <v>-471</v>
       </c>
       <c r="C35" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1913,15 +1958,15 @@
       </c>
       <c r="D35" s="1">
         <f ca="1">IF(C35 = 0.6, G34, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E35" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-14</v>
+        <v>210</v>
       </c>
       <c r="G35" s="35"/>
     </row>
@@ -1931,7 +1976,7 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-14</v>
+        <v>210</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
@@ -1940,15 +1985,15 @@
       </c>
       <c r="E36" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>285</v>
+        <v>330</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-299</v>
+        <v>-120</v>
       </c>
       <c r="G36" s="35">
-        <f ca="1">IF(F36 &lt; J29, (J28-F36), 0 )</f>
-        <v>1299</v>
+        <f ca="1">IF(F36 &lt; J29, (IF(F36&lt;0, J28, J28-F36)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -1957,23 +2002,23 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-299</v>
+        <v>-120</v>
       </c>
       <c r="C37" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D37" s="1">
         <f ca="1">IF(C37 = 0.6, G36, 0)</f>
-        <v>1299</v>
+        <v>0</v>
       </c>
       <c r="E37" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>631</v>
+        <v>-476</v>
       </c>
       <c r="G37" s="35"/>
     </row>
@@ -1983,24 +2028,24 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>631</v>
+        <v>-476</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
         <f ca="1">IF(C37 = 0.4, G36, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E38" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>350</v>
+        <v>313</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>281</v>
+        <v>211</v>
       </c>
       <c r="G38" s="35">
-        <f ca="1">IF(F38 &lt; J29, (J28-F38), 0 )</f>
-        <v>719</v>
+        <f ca="1">IF(F38 &lt; J29, (IF(F38&lt;0, J28, J28-F38)), 0 )</f>
+        <v>789</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2009,7 +2054,7 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>281</v>
+        <v>211</v>
       </c>
       <c r="C39" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2017,15 +2062,15 @@
       </c>
       <c r="D39" s="1">
         <f ca="1">IF(C39 = 0.6, G38, 0)</f>
-        <v>719</v>
+        <v>789</v>
       </c>
       <c r="E39" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>676</v>
+        <v>664</v>
       </c>
       <c r="G39" s="35"/>
     </row>
@@ -2035,7 +2080,7 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>676</v>
+        <v>664</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1">
@@ -2044,15 +2089,15 @@
       </c>
       <c r="E40" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>381</v>
+        <v>312</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>295</v>
+        <v>352</v>
       </c>
       <c r="G40" s="35">
-        <f ca="1">IF(F40 &lt; J29, (J28-F40), 0 )</f>
-        <v>705</v>
+        <f ca="1">IF(F40 &lt; J29, (IF(F40&lt;0, J28, J28-F40)), 0 )</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2061,7 +2106,7 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>295</v>
+        <v>352</v>
       </c>
       <c r="C41" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2073,11 +2118,11 @@
       </c>
       <c r="E41" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>322</v>
+        <v>377</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-27</v>
+        <v>-25</v>
       </c>
       <c r="G41" s="35"/>
     </row>
@@ -2087,24 +2132,24 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-27</v>
+        <v>-25</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1">
         <f ca="1">IF(C41 = 0.4, G40, 0)</f>
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="E42" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>259</v>
+        <v>364</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>419</v>
+        <v>-389</v>
       </c>
       <c r="G42" s="35">
-        <f ca="1">IF(F42 &lt; J29, (J28-F42), 0 )</f>
-        <v>0</v>
+        <f ca="1">IF(F42 &lt; J29, (IF(F42&lt;0, J28, J28-F42)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2113,11 +2158,11 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>419</v>
+        <v>-389</v>
       </c>
       <c r="C43" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D43" s="1">
         <f ca="1">IF(C43 = 0.6, G42, 0)</f>
@@ -2125,11 +2170,11 @@
       </c>
       <c r="E43" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>409</v>
+        <v>356</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>-745</v>
       </c>
       <c r="G43" s="35"/>
     </row>
@@ -2139,24 +2184,24 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>-745</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1">
         <f ca="1">IF(C43 = 0.4, G42, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E44" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>304</v>
+        <v>334</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-294</v>
+        <v>-79</v>
       </c>
       <c r="G44" s="35">
-        <f ca="1">IF(F44 &lt; J29, (J28-F44), 0 )</f>
-        <v>1294</v>
+        <f ca="1">IF(F44 &lt; J29, (IF(F44&lt;0, J28, J28-F44)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2165,7 +2210,7 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-294</v>
+        <v>-79</v>
       </c>
       <c r="C45" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2177,11 +2222,11 @@
       </c>
       <c r="E45" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>296</v>
+        <v>353</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-590</v>
+        <v>-432</v>
       </c>
       <c r="G45" s="35"/>
     </row>
@@ -2191,24 +2236,24 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-590</v>
+        <v>-432</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1">
         <f ca="1">IF(C45 = 0.4, G44, 0)</f>
-        <v>1294</v>
+        <v>1000</v>
       </c>
       <c r="E46" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>311</v>
+        <v>359</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>393</v>
+        <v>209</v>
       </c>
       <c r="G46" s="35">
-        <f ca="1">IF(F46 &lt; J29, (J28-F46), 0 )</f>
-        <v>0</v>
+        <f ca="1">IF(F46 &lt; J29, (IF(F46&lt;0, J28, J28-F46)), 0 )</f>
+        <v>791</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2217,11 +2262,11 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>393</v>
+        <v>209</v>
       </c>
       <c r="C47" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D47" s="1">
         <f ca="1">IF(C47 = 0.6, G46, 0)</f>
@@ -2229,11 +2274,11 @@
       </c>
       <c r="E47" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>-141</v>
       </c>
       <c r="G47" s="35"/>
     </row>
@@ -2243,24 +2288,24 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>-141</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
         <f ca="1">IF(C47 = 0.4, G46, 0)</f>
-        <v>0</v>
+        <v>791</v>
       </c>
       <c r="E48" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>345</v>
+        <v>389</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-259</v>
+        <v>261</v>
       </c>
       <c r="G48" s="35">
-        <f ca="1">IF(F48 &lt; J29, (J28-F48), 0 )</f>
-        <v>1259</v>
+        <f ca="1">IF(F48 &lt; J29, (IF(F48&lt;0, J28, J28-F48)), 0 )</f>
+        <v>739</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2269,23 +2314,23 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-259</v>
+        <v>261</v>
       </c>
       <c r="C49" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D49" s="1">
         <f ca="1">IF(C49 = 0.6, G48, 0)</f>
-        <v>0</v>
+        <v>739</v>
       </c>
       <c r="E49" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-578</v>
+        <v>659</v>
       </c>
       <c r="G49" s="35"/>
     </row>
@@ -2295,24 +2340,24 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-578</v>
+        <v>659</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1">
         <f ca="1">IF(C49 = 0.4, G48, 0)</f>
-        <v>1259</v>
+        <v>0</v>
       </c>
       <c r="E50" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>402</v>
+        <v>346</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>279</v>
+        <v>313</v>
       </c>
       <c r="G50" s="35">
-        <f ca="1">IF(F50 &lt; J29, (J28-F50), 0 )</f>
-        <v>721</v>
+        <f ca="1">IF(F50 &lt; J29, (IF(F50&lt;0, J28, J28-F50)), 0 )</f>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2321,7 +2366,7 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>279</v>
+        <v>313</v>
       </c>
       <c r="C51" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2333,11 +2378,11 @@
       </c>
       <c r="E51" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-63</v>
+        <v>-47</v>
       </c>
       <c r="G51" s="35"/>
     </row>
@@ -2347,24 +2392,24 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-63</v>
+        <v>-47</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1">
         <f ca="1">IF(C51 = 0.4, G50, 0)</f>
-        <v>721</v>
+        <v>0</v>
       </c>
       <c r="E52" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>316</v>
+        <v>-400</v>
       </c>
       <c r="G52" s="35">
-        <f ca="1">IF(F52 &lt; J29, (J28-F52), 0 )</f>
-        <v>0</v>
+        <f ca="1">IF(F52 &lt; J29, (IF(F52&lt;0, J28, J28-F52)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2373,7 +2418,7 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>316</v>
+        <v>-400</v>
       </c>
       <c r="C53" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2385,11 +2430,11 @@
       </c>
       <c r="E53" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-12</v>
+        <v>-725</v>
       </c>
       <c r="G53" s="35"/>
     </row>
@@ -2399,36 +2444,36 @@
       </c>
       <c r="B54" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>-12</v>
+        <v>-725</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
         <f ca="1">IF(C53 = 0.4, G52, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E54" s="33">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>354</v>
+        <v>378</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>-366</v>
+        <v>-103</v>
       </c>
       <c r="G54" s="36">
-        <f ca="1">IF(F54 &lt; J29, (J28-F54), 0 )</f>
-        <v>1366</v>
+        <f ca="1">IF(F54 &lt; J29, (IF(F54&lt;0, J28, J28-F54)), 0 )</f>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K17:L17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
inicio 2) + inicio relatorio
</commit_message>
<xml_diff>
--- a/Previsao.xlsx
+++ b/Previsao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogobraga/Desktop/InventoryManagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FB9CFB-AA39-F74F-94BA-1C274D26010F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF212C5-583C-5D45-A224-9494BCD33E28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{0D2C59F3-1D13-48BD-903E-89ECABAE3337}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>PERÍODO</t>
   </si>
@@ -132,6 +133,9 @@
   </si>
   <si>
     <t>CASO DE QUEBRA DE INVENTARIO</t>
+  </si>
+  <si>
+    <t>Nº TENTATIVA</t>
   </si>
 </sst>
 </file>
@@ -218,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -506,11 +510,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -612,34 +655,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -956,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002CE9F5-C0CF-6F4A-9226-C15012BC27ED}">
-  <dimension ref="A2:M54"/>
+  <dimension ref="A2:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1010,7 +1068,7 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29">
         <f ca="1">INT(RANDBETWEEN(347,575))</f>
-        <v>528</v>
+        <v>411</v>
       </c>
       <c r="G4" s="34"/>
     </row>
@@ -1020,17 +1078,17 @@
       </c>
       <c r="B5" s="1">
         <f ca="1">F4</f>
-        <v>528</v>
+        <v>411</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F5" s="1">
         <f ca="1">B5-E5+D5</f>
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="G5" s="35"/>
       <c r="I5" s="6" t="s">
@@ -1049,17 +1107,17 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B54" ca="1" si="0">F5</f>
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6:F54" ca="1" si="1">B6-E6+D6</f>
-        <v>-315</v>
+        <v>-446</v>
       </c>
       <c r="G6" s="35">
         <f ca="1">IF(F6 &lt; J29, (IF(F6&lt;0, J28, J28-F6)), 0 )</f>
@@ -1081,23 +1139,23 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-315</v>
+        <v>-446</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">IF(C7 = 0.6, G6, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E7" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>348</v>
+        <v>406</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>337</v>
+        <v>-852</v>
       </c>
       <c r="G7" s="35"/>
       <c r="I7" s="9" t="s">
@@ -1116,20 +1174,20 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>337</v>
+        <v>-852</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <f ca="1">IF(C7 = 0.4, G6, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>465</v>
+        <v>484</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-128</v>
+        <v>-336</v>
       </c>
       <c r="G8" s="35">
         <f ca="1">IF(F8 &lt; J29, (IF(F8&lt;0, J28, J28-F8)), 0 )</f>
@@ -1151,7 +1209,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-128</v>
+        <v>-336</v>
       </c>
       <c r="C9" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1163,11 +1221,11 @@
       </c>
       <c r="E9" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>390</v>
+        <v>440</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>482</v>
+        <v>224</v>
       </c>
       <c r="G9" s="35"/>
     </row>
@@ -1177,7 +1235,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>482</v>
+        <v>224</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
@@ -1186,15 +1244,15 @@
       </c>
       <c r="E10" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>-229</v>
       </c>
       <c r="G10" s="35">
         <f ca="1">IF(F10 &lt; J29, (IF(F10&lt;0, J28, J28-F10)), 0 )</f>
-        <v>963</v>
+        <v>1000</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>11</v>
@@ -1209,23 +1267,23 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>-229</v>
       </c>
       <c r="C11" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D11" s="1">
         <f ca="1">IF(C11 = 0.6, G10, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E11" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>385</v>
+        <v>450</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-348</v>
+        <v>321</v>
       </c>
       <c r="G11" s="35"/>
       <c r="I11" s="9">
@@ -1241,24 +1299,24 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-348</v>
+        <v>321</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
         <f ca="1">IF(C11 = 0.4, G10, 0)</f>
-        <v>963</v>
+        <v>0</v>
       </c>
       <c r="E12" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>461</v>
+        <v>529</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>154</v>
+        <v>-208</v>
       </c>
       <c r="G12" s="35">
         <f ca="1">IF(F12 &lt; J29, (IF(F12&lt;0, J28, J28-F12)), 0 )</f>
-        <v>846</v>
+        <v>1000</v>
       </c>
       <c r="I12" s="11">
         <v>2</v>
@@ -1273,23 +1331,23 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>154</v>
+        <v>-208</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D13" s="1">
         <f ca="1">IF(C13 = 0.6, G12, 0)</f>
-        <v>846</v>
+        <v>0</v>
       </c>
       <c r="E13" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>406</v>
+        <v>436</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>594</v>
+        <v>-644</v>
       </c>
       <c r="G13" s="35"/>
     </row>
@@ -1299,24 +1357,24 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>594</v>
+        <v>-644</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <f ca="1">IF(C13 = 0.4, G12, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>382</v>
+        <v>537</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>212</v>
+        <v>-181</v>
       </c>
       <c r="G14" s="35">
         <f ca="1">IF(F14 &lt; J29, (IF(F14&lt;0, J28, J28-F14)), 0 )</f>
-        <v>788</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -1325,7 +1383,7 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>212</v>
+        <v>-181</v>
       </c>
       <c r="C15" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1333,15 +1391,15 @@
       </c>
       <c r="D15" s="1">
         <f ca="1">IF(C15 = 0.6, G14, 0)</f>
-        <v>788</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>478</v>
+        <v>436</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>522</v>
+        <v>383</v>
       </c>
       <c r="G15" s="35"/>
       <c r="M15" s="15"/>
@@ -1352,7 +1410,7 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>522</v>
+        <v>383</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
@@ -1361,15 +1419,15 @@
       </c>
       <c r="E16" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>-87</v>
       </c>
       <c r="G16" s="35">
         <f ca="1">IF(F16 &lt; J29, (IF(F16&lt;0, J28, J28-F16)), 0 )</f>
-        <v>928</v>
+        <v>1000</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>15</v>
@@ -1377,10 +1435,10 @@
       <c r="J16" s="21">
         <v>96.5</v>
       </c>
-      <c r="K16" s="37" t="s">
+      <c r="K16" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="38"/>
+      <c r="L16" s="45"/>
     </row>
     <row r="17" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
@@ -1388,7 +1446,7 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>-87</v>
       </c>
       <c r="C17" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1396,15 +1454,15 @@
       </c>
       <c r="D17" s="1">
         <f ca="1">IF(C17 = 0.6, G16, 0)</f>
-        <v>928</v>
+        <v>1000</v>
       </c>
       <c r="E17" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>354</v>
+        <v>469</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>646</v>
+        <v>444</v>
       </c>
       <c r="G17" s="35"/>
       <c r="I17" s="17" t="s">
@@ -1413,10 +1471,10 @@
       <c r="J17" s="21">
         <v>0.18</v>
       </c>
-      <c r="K17" s="39" t="s">
+      <c r="K17" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="39"/>
+      <c r="L17" s="43"/>
     </row>
     <row r="18" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
@@ -1424,7 +1482,7 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>646</v>
+        <v>444</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
@@ -1433,15 +1491,15 @@
       </c>
       <c r="E18" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>425</v>
+        <v>455</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>221</v>
+        <v>-11</v>
       </c>
       <c r="G18" s="35">
         <f ca="1">IF(F18 &lt; J29, (IF(F18&lt;0, J28, J28-F18)), 0 )</f>
-        <v>779</v>
+        <v>1000</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>19</v>
@@ -1450,10 +1508,10 @@
         <f>J16*J17</f>
         <v>17.37</v>
       </c>
-      <c r="K18" s="37" t="s">
+      <c r="K18" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="39"/>
+      <c r="L18" s="43"/>
     </row>
     <row r="19" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
@@ -1461,7 +1519,7 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>221</v>
+        <v>-11</v>
       </c>
       <c r="C19" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1469,15 +1527,15 @@
       </c>
       <c r="D19" s="1">
         <f ca="1">IF(C19 = 0.6, G18, 0)</f>
-        <v>779</v>
+        <v>1000</v>
       </c>
       <c r="E19" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>442</v>
+        <v>389</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>558</v>
+        <v>600</v>
       </c>
       <c r="G19" s="35"/>
     </row>
@@ -1487,7 +1545,7 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>558</v>
+        <v>600</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
@@ -1496,15 +1554,15 @@
       </c>
       <c r="E20" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>370</v>
+        <v>482</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="G20" s="35">
         <f ca="1">IF(F20 &lt; J29, (IF(F20&lt;0, J28, J28-F20)), 0 )</f>
-        <v>812</v>
+        <v>882</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>13</v>
@@ -1524,23 +1582,23 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="C21" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D21" s="1">
         <f ca="1">IF(C21 = 0.6, G20, 0)</f>
-        <v>812</v>
+        <v>0</v>
       </c>
       <c r="E21" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>592</v>
+        <v>632</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>408</v>
+        <v>-514</v>
       </c>
       <c r="G21" s="35"/>
       <c r="I21" s="20" t="s">
@@ -1550,10 +1608,10 @@
         <f>20+2*J20</f>
         <v>34</v>
       </c>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="42"/>
+      <c r="L21" s="40"/>
     </row>
     <row r="22" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
@@ -1561,20 +1619,20 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>408</v>
+        <v>-514</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <f ca="1">IF(C21 = 0.4, G20, 0)</f>
-        <v>0</v>
+        <v>882</v>
       </c>
       <c r="E22" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>536</v>
+        <v>600</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-128</v>
+        <v>-232</v>
       </c>
       <c r="G22" s="35">
         <f ca="1">IF(F22 &lt; J29, (IF(F22&lt;0, J28, J28-F22)), 0 )</f>
@@ -1582,8 +1640,8 @@
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
     </row>
     <row r="23" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
@@ -1591,23 +1649,23 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-128</v>
+        <v>-232</v>
       </c>
       <c r="C23" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D23" s="1">
         <f ca="1">IF(C23 = 0.6, G22, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E23" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>571</v>
+        <v>585</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-699</v>
+        <v>183</v>
       </c>
       <c r="G23" s="35"/>
       <c r="I23" s="17" t="s">
@@ -1616,10 +1674,10 @@
       <c r="J23" s="21">
         <v>900</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="L23" s="42"/>
+      <c r="L23" s="40"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -1628,20 +1686,20 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-699</v>
+        <v>183</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <f ca="1">IF(C23 = 0.4, G22, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E24" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-257</v>
+        <v>-361</v>
       </c>
       <c r="G24" s="35">
         <f ca="1">IF(F24 &lt; J29, (IF(F24&lt;0, J28, J28-F24)), 0 )</f>
@@ -1658,7 +1716,7 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-257</v>
+        <v>-361</v>
       </c>
       <c r="C25" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1670,11 +1728,11 @@
       </c>
       <c r="E25" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>591</v>
+        <v>562</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="G25" s="35"/>
       <c r="I25" s="20" t="s">
@@ -1683,10 +1741,10 @@
       <c r="J25" s="21">
         <v>2</v>
       </c>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="42"/>
+      <c r="L25" s="40"/>
     </row>
     <row r="26" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
@@ -1694,7 +1752,7 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
@@ -1703,11 +1761,11 @@
       </c>
       <c r="E26" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>571</v>
+        <v>640</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-419</v>
+        <v>-563</v>
       </c>
       <c r="G26" s="35">
         <f ca="1">IF(F26 &lt; J29, (IF(F26&lt;0, J28, J28-F26)), 0 )</f>
@@ -1720,29 +1778,29 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-419</v>
+        <v>-563</v>
       </c>
       <c r="C27" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D27" s="1">
         <f ca="1">IF(C27 = 0.6, G26, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E27" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>527</v>
+        <v>558</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-946</v>
+        <v>-121</v>
       </c>
       <c r="G27" s="35"/>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="44"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:13" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
@@ -1750,20 +1808,20 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-946</v>
+        <v>-121</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
         <f ca="1">IF(C27 = 0.4, G26, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E28" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>556</v>
+        <v>496</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-502</v>
+        <v>-617</v>
       </c>
       <c r="G28" s="35">
         <f ca="1">IF(F28 &lt; J29, (IF(F28&lt;0, J28, J28-F28)), 0 )</f>
@@ -1782,23 +1840,23 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-502</v>
+        <v>-617</v>
       </c>
       <c r="C29" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D29" s="1">
         <f ca="1">IF(C29 = 0.6, G28, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E29" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>540</v>
+        <v>596</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-1042</v>
+        <v>-213</v>
       </c>
       <c r="G29" s="35"/>
       <c r="I29" s="11" t="s">
@@ -1814,20 +1872,20 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1042</v>
+        <v>-213</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <f ca="1">IF(C29 = 0.4, G28, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E30" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>540</v>
+        <v>577</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-582</v>
+        <v>-790</v>
       </c>
       <c r="G30" s="35">
         <f ca="1">IF(F30 &lt; J29, (IF(F30&lt;0, J28, J28-F30)), 0 )</f>
@@ -1840,29 +1898,29 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-582</v>
+        <v>-790</v>
       </c>
       <c r="C31" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D31" s="1">
         <f ca="1">IF(C31 = 0.6, G30, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E31" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>622</v>
+        <v>479</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-204</v>
+        <v>-1269</v>
       </c>
       <c r="G31" s="35"/>
-      <c r="I31" s="45" t="s">
+      <c r="I31" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="46" t="s">
+      <c r="J31" s="38" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1872,20 +1930,20 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-204</v>
+        <v>-1269</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
         <f ca="1">IF(C31 = 0.4, G30, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E32" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>540</v>
+        <v>625</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-744</v>
+        <v>-894</v>
       </c>
       <c r="G32" s="35">
         <f ca="1">IF(F32 &lt; J29, (IF(F32&lt;0, J28, J28-F32)), 0 )</f>
@@ -1898,7 +1956,7 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-744</v>
+        <v>-894</v>
       </c>
       <c r="C33" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1910,11 +1968,11 @@
       </c>
       <c r="E33" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>371</v>
+        <v>294</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-115</v>
+        <v>-188</v>
       </c>
       <c r="G33" s="35"/>
     </row>
@@ -1924,7 +1982,7 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-115</v>
+        <v>-188</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
@@ -1937,7 +1995,7 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-471</v>
+        <v>-544</v>
       </c>
       <c r="G34" s="35">
         <f ca="1">IF(F34 &lt; J29, (IF(F34&lt;0, J28, J28-F34)), 0 )</f>
@@ -1950,23 +2008,23 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-471</v>
+        <v>-544</v>
       </c>
       <c r="C35" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D35" s="1">
         <f ca="1">IF(C35 = 0.6, G34, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E35" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>210</v>
+        <v>-875</v>
       </c>
       <c r="G35" s="35"/>
     </row>
@@ -1976,20 +2034,20 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>-875</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
         <f ca="1">IF(C35 = 0.4, G34, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E36" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-120</v>
+        <v>-219</v>
       </c>
       <c r="G36" s="35">
         <f ca="1">IF(F36 &lt; J29, (IF(F36&lt;0, J28, J28-F36)), 0 )</f>
@@ -2002,7 +2060,7 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-120</v>
+        <v>-219</v>
       </c>
       <c r="C37" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2014,11 +2072,11 @@
       </c>
       <c r="E37" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-476</v>
+        <v>-552</v>
       </c>
       <c r="G37" s="35"/>
     </row>
@@ -2028,7 +2086,7 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-476</v>
+        <v>-552</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
@@ -2037,15 +2095,15 @@
       </c>
       <c r="E38" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>313</v>
+        <v>338</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>211</v>
+        <v>110</v>
       </c>
       <c r="G38" s="35">
         <f ca="1">IF(F38 &lt; J29, (IF(F38&lt;0, J28, J28-F38)), 0 )</f>
-        <v>789</v>
+        <v>890</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2054,23 +2112,23 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>211</v>
+        <v>110</v>
       </c>
       <c r="C39" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D39" s="1">
         <f ca="1">IF(C39 = 0.6, G38, 0)</f>
-        <v>789</v>
+        <v>0</v>
       </c>
       <c r="E39" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>664</v>
+        <v>-240</v>
       </c>
       <c r="G39" s="35"/>
     </row>
@@ -2080,20 +2138,20 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>664</v>
+        <v>-240</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1">
         <f ca="1">IF(C39 = 0.4, G38, 0)</f>
-        <v>0</v>
+        <v>890</v>
       </c>
       <c r="E40" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>312</v>
+        <v>348</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>352</v>
+        <v>302</v>
       </c>
       <c r="G40" s="35">
         <f ca="1">IF(F40 &lt; J29, (IF(F40&lt;0, J28, J28-F40)), 0 )</f>
@@ -2106,7 +2164,7 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>352</v>
+        <v>302</v>
       </c>
       <c r="C41" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2118,11 +2176,11 @@
       </c>
       <c r="E41" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>377</v>
+        <v>326</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-25</v>
+        <v>-24</v>
       </c>
       <c r="G41" s="35"/>
     </row>
@@ -2132,7 +2190,7 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-25</v>
+        <v>-24</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1">
@@ -2141,11 +2199,11 @@
       </c>
       <c r="E42" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>364</v>
+        <v>295</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-389</v>
+        <v>-319</v>
       </c>
       <c r="G42" s="35">
         <f ca="1">IF(F42 &lt; J29, (IF(F42&lt;0, J28, J28-F42)), 0 )</f>
@@ -2158,23 +2216,23 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-389</v>
+        <v>-319</v>
       </c>
       <c r="C43" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D43" s="1">
         <f ca="1">IF(C43 = 0.6, G42, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E43" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>356</v>
+        <v>417</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-745</v>
+        <v>264</v>
       </c>
       <c r="G43" s="35"/>
     </row>
@@ -2184,20 +2242,20 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-745</v>
+        <v>264</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1">
         <f ca="1">IF(C43 = 0.4, G42, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E44" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-79</v>
+        <v>-82</v>
       </c>
       <c r="G44" s="35">
         <f ca="1">IF(F44 &lt; J29, (IF(F44&lt;0, J28, J28-F44)), 0 )</f>
@@ -2210,23 +2268,23 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-79</v>
+        <v>-82</v>
       </c>
       <c r="C45" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D45" s="1">
         <f ca="1">IF(C45 = 0.6, G44, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E45" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-432</v>
+        <v>567</v>
       </c>
       <c r="G45" s="35"/>
     </row>
@@ -2236,24 +2294,24 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-432</v>
+        <v>567</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1">
         <f ca="1">IF(C45 = 0.4, G44, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E46" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="G46" s="35">
         <f ca="1">IF(F46 &lt; J29, (IF(F46&lt;0, J28, J28-F46)), 0 )</f>
-        <v>791</v>
+        <v>815</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2262,7 +2320,7 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="C47" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2274,11 +2332,11 @@
       </c>
       <c r="E47" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>350</v>
+        <v>380</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-141</v>
+        <v>-195</v>
       </c>
       <c r="G47" s="35"/>
     </row>
@@ -2288,24 +2346,24 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-141</v>
+        <v>-195</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
         <f ca="1">IF(C47 = 0.4, G46, 0)</f>
-        <v>791</v>
+        <v>815</v>
       </c>
       <c r="E48" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>389</v>
+        <v>308</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="G48" s="35">
         <f ca="1">IF(F48 &lt; J29, (IF(F48&lt;0, J28, J28-F48)), 0 )</f>
-        <v>739</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2314,23 +2372,23 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="C49" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D49" s="1">
         <f ca="1">IF(C49 = 0.6, G48, 0)</f>
-        <v>739</v>
+        <v>0</v>
       </c>
       <c r="E49" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>659</v>
+        <v>-22</v>
       </c>
       <c r="G49" s="35"/>
     </row>
@@ -2340,7 +2398,7 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>659</v>
+        <v>-22</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1">
@@ -2349,15 +2407,15 @@
       </c>
       <c r="E50" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>313</v>
+        <v>-352</v>
       </c>
       <c r="G50" s="35">
         <f ca="1">IF(F50 &lt; J29, (IF(F50&lt;0, J28, J28-F50)), 0 )</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2366,23 +2424,23 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>313</v>
+        <v>-352</v>
       </c>
       <c r="C51" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D51" s="1">
         <f ca="1">IF(C51 = 0.6, G50, 0)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E51" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>360</v>
+        <v>279</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-47</v>
+        <v>369</v>
       </c>
       <c r="G51" s="35"/>
     </row>
@@ -2392,7 +2450,7 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-47</v>
+        <v>369</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1">
@@ -2401,11 +2459,11 @@
       </c>
       <c r="E52" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>353</v>
+        <v>378</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-400</v>
+        <v>-9</v>
       </c>
       <c r="G52" s="35">
         <f ca="1">IF(F52 &lt; J29, (IF(F52&lt;0, J28, J28-F52)), 0 )</f>
@@ -2418,7 +2476,7 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-400</v>
+        <v>-9</v>
       </c>
       <c r="C53" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2430,11 +2488,11 @@
       </c>
       <c r="E53" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>-725</v>
+        <v>-342</v>
       </c>
       <c r="G53" s="35"/>
     </row>
@@ -2444,7 +2502,7 @@
       </c>
       <c r="B54" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>-725</v>
+        <v>-342</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
@@ -2453,15 +2511,152 @@
       </c>
       <c r="E54" s="33">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>-103</v>
+        <v>307</v>
       </c>
       <c r="G54" s="36">
         <f ca="1">IF(F54 &lt; J29, (IF(F54&lt;0, J28, J28-F54)), 0 )</f>
-        <v>1000</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="49">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="49">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="49">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="49">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="49">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="49">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="49">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="49">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="49">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="49">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="50">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trabalho quase quase acabado
</commit_message>
<xml_diff>
--- a/Previsao.xlsx
+++ b/Previsao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Desktop/Desktop_iCloud/Universidade/3ºano/2ºsemestre/MEIO/InventoryManagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A28814-D3DB-CC4D-A3CA-3A8DB4CE991D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2901E529-53F2-9A46-BEF0-D89CE21E0274}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0D2C59F3-1D13-48BD-903E-89ECABAE3337}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>PERÍODO</t>
   </si>
@@ -114,9 +114,6 @@
     <t>* ciclo de encomenda</t>
   </si>
   <si>
-    <t>PARÂMETROS VARIÁVEIS</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -153,32 +150,65 @@
     <t>P[DDPP&gt;S]</t>
   </si>
   <si>
-    <t>MÉDIA DDPP</t>
-  </si>
-  <si>
-    <t>DESVIO DDPP</t>
-  </si>
-  <si>
     <t>Desvio Anual</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
     <t>E[DDPP&gt;S]</t>
   </si>
   <si>
     <t>Custos totais</t>
+  </si>
+  <si>
+    <t>PARÂMETROS VARIÁVEIS [1,16]</t>
+  </si>
+  <si>
+    <t>PARÂMETROS VARIÁVEIS [17,28]</t>
+  </si>
+  <si>
+    <t>PARÂMETROS VARIÁVEIS [29,50]</t>
+  </si>
+  <si>
+    <t>Média DDPP[1,16]</t>
+  </si>
+  <si>
+    <t>Desvio DDPP[1,16]</t>
+  </si>
+  <si>
+    <t>Média DDPP[17,28]</t>
+  </si>
+  <si>
+    <t>Desvio DDPP[17,28]</t>
+  </si>
+  <si>
+    <t>Média DDPP[29,50]</t>
+  </si>
+  <si>
+    <t>Desvio DDPP[29,50]</t>
+  </si>
+  <si>
+    <t>P[DDPP&gt;S] [1,16]</t>
+  </si>
+  <si>
+    <t>P[DDPP&gt;S] [17,28]</t>
+  </si>
+  <si>
+    <t>P[DDPP&gt;S] [29,50]</t>
+  </si>
+  <si>
+    <t>Z[1,16]</t>
+  </si>
+  <si>
+    <t>Z[17,28]</t>
+  </si>
+  <si>
+    <t>Z[29,50]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +249,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,8 +311,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -609,11 +681,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -688,9 +843,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,6 +887,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,29 +930,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1098,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002CE9F5-C0CF-6F4A-9226-C15012BC27ED}">
-  <dimension ref="A2:N84"/>
+  <dimension ref="A2:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1116,8 +1312,12 @@
     <col min="9" max="9" width="26.83203125" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="17" max="17" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1138,25 +1338,25 @@
         <v>4</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>0</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29">
-        <f ca="1">INT(RANDBETWEEN(347,575))</f>
-        <v>568</v>
-      </c>
-      <c r="G4" s="34"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28">
+        <f ca="1">INT(RANDBETWEEN(J29,J28))</f>
+        <v>1342</v>
+      </c>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
@@ -1164,19 +1364,19 @@
       </c>
       <c r="B5" s="1">
         <f ca="1">IF(F4 &gt; 0, F4, 0)</f>
-        <v>568</v>
+        <v>1342</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>371</v>
+        <v>399</v>
       </c>
       <c r="F5" s="1">
         <f ca="1">B5-E5+D5</f>
-        <v>197</v>
-      </c>
-      <c r="G5" s="35"/>
+        <v>943</v>
+      </c>
+      <c r="G5" s="34"/>
       <c r="I5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1186,35 +1386,35 @@
       <c r="K5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="58">
-        <f>AVERAGE(J6,J7,J8)</f>
-        <v>452.5333333333333</v>
+      <c r="M5" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="47">
+        <f>(J6*16 + J7 *12+ J8*22)/50</f>
+        <v>430.08839999999998</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="A6" s="57">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B54" ca="1" si="0">IF(F5 &gt; 0, F5, 0)</f>
-        <v>197</v>
+        <v>943</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>393</v>
+        <v>483</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6:F54" ca="1" si="1">B6-E6+D6</f>
-        <v>-196</v>
-      </c>
-      <c r="G6" s="35">
+        <v>460</v>
+      </c>
+      <c r="G6" s="34">
         <f ca="1">IF(F6 &lt; J29, (IF(F6&lt;0, J28, J28-F6)), 0 )</f>
-        <v>1664</v>
+        <v>1031</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>7</v>
@@ -1225,12 +1425,12 @@
       <c r="K6" s="10">
         <v>37.85</v>
       </c>
-      <c r="M6" s="52" t="s">
-        <v>42</v>
+      <c r="M6" s="43" t="s">
+        <v>39</v>
       </c>
       <c r="N6" s="21">
         <f>N5*0.087</f>
-        <v>39.370399999999997</v>
+        <v>37.417690799999995</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="19" x14ac:dyDescent="0.2">
@@ -1239,25 +1439,25 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>460</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">IF(C7 = 0.6, G6, 0)</f>
-        <v>1664</v>
-      </c>
-      <c r="E7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>438</v>
+        <v>343</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1226</v>
-      </c>
-      <c r="G7" s="35"/>
+        <v>117</v>
+      </c>
+      <c r="G7" s="34"/>
       <c r="I7" s="9" t="s">
         <v>8</v>
       </c>
@@ -1269,29 +1469,29 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="57">
         <v>4</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1226</v>
+        <v>117</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <f ca="1">IF(C7 = 0.4, G6, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="30">
+        <v>1031</v>
+      </c>
+      <c r="E8" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>351</v>
+        <v>417</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>875</v>
-      </c>
-      <c r="G8" s="35">
+        <v>731</v>
+      </c>
+      <c r="G8" s="34">
         <f ca="1">IF(F8 &lt; J29, (IF(F8&lt;0, J28, J28-F8)), 0 )</f>
-        <v>789</v>
+        <v>760</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>9</v>
@@ -1309,7 +1509,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>875</v>
+        <v>731</v>
       </c>
       <c r="C9" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1319,40 +1519,40 @@
         <f ca="1">IF(C9 = 0.6, G8, 0)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>414</v>
+        <v>451</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>461</v>
-      </c>
-      <c r="G9" s="35"/>
+        <v>280</v>
+      </c>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:14" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="27">
+      <c r="A10" s="57">
         <v>6</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>461</v>
+        <v>280</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
         <f ca="1">IF(C9 = 0.4, G8, 0)</f>
-        <v>789</v>
-      </c>
-      <c r="E10" s="30">
+        <v>760</v>
+      </c>
+      <c r="E10" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>424</v>
+        <v>452</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>826</v>
-      </c>
-      <c r="G10" s="35">
+        <v>588</v>
+      </c>
+      <c r="G10" s="34">
         <f ca="1">IF(F10 &lt; J29, (IF(F10&lt;0, J28, J28-F10)), 0 )</f>
-        <v>838</v>
+        <v>903</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>11</v>
@@ -1367,7 +1567,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>826</v>
+        <v>588</v>
       </c>
       <c r="C11" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1375,17 +1575,17 @@
       </c>
       <c r="D11" s="1">
         <f ca="1">IF(C11 = 0.6, G10, 0)</f>
-        <v>838</v>
-      </c>
-      <c r="E11" s="30">
+        <v>903</v>
+      </c>
+      <c r="E11" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>377</v>
+        <v>331</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1287</v>
-      </c>
-      <c r="G11" s="35"/>
+        <v>1160</v>
+      </c>
+      <c r="G11" s="34"/>
       <c r="I11" s="9">
         <v>1</v>
       </c>
@@ -1394,29 +1594,29 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="A12" s="57">
         <v>8</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1287</v>
+        <v>1160</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
         <f ca="1">IF(C11 = 0.4, G10, 0)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>882</v>
-      </c>
-      <c r="G12" s="35">
+        <v>752</v>
+      </c>
+      <c r="G12" s="34">
         <f ca="1">IF(F12 &lt; J29, (IF(F12&lt;0, J28, J28-F12)), 0 )</f>
-        <v>782</v>
+        <v>739</v>
       </c>
       <c r="I12" s="11">
         <v>2</v>
@@ -1431,50 +1631,50 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>882</v>
+        <v>752</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D13" s="1">
         <f ca="1">IF(C13 = 0.6, G12, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="30">
+        <v>739</v>
+      </c>
+      <c r="E13" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>381</v>
+        <v>473</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>501</v>
-      </c>
-      <c r="G13" s="35"/>
+        <v>1018</v>
+      </c>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:14" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="27">
+      <c r="A14" s="57">
         <v>10</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>501</v>
+        <v>1018</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <f ca="1">IF(C13 = 0.4, G12, 0)</f>
-        <v>782</v>
-      </c>
-      <c r="E14" s="30">
+        <v>0</v>
+      </c>
+      <c r="E14" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>862</v>
-      </c>
-      <c r="G14" s="35">
+        <v>612</v>
+      </c>
+      <c r="G14" s="34">
         <f ca="1">IF(F14 &lt; J29, (IF(F14&lt;0, J28, J28-F14)), 0 )</f>
-        <v>802</v>
+        <v>879</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -1483,51 +1683,51 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>862</v>
+        <v>612</v>
       </c>
       <c r="C15" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D15" s="1">
         <f ca="1">IF(C15 = 0.6, G14, 0)</f>
-        <v>802</v>
-      </c>
-      <c r="E15" s="30">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1192</v>
-      </c>
-      <c r="G15" s="35"/>
+        <v>153</v>
+      </c>
+      <c r="G15" s="34"/>
       <c r="M15" s="15"/>
     </row>
     <row r="16" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
+      <c r="A16" s="57">
         <v>12</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1192</v>
+        <v>153</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <f ca="1">IF(C15 = 0.4, G14, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="30">
+        <v>879</v>
+      </c>
+      <c r="E16" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>733</v>
-      </c>
-      <c r="G16" s="35">
+        <v>590</v>
+      </c>
+      <c r="G16" s="34">
         <f ca="1">IF(F16 &lt; J29, (IF(F16&lt;0, J28, J28-F16)), 0 )</f>
-        <v>931</v>
+        <v>901</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>15</v>
@@ -1535,18 +1735,18 @@
       <c r="J16" s="21">
         <v>96.5</v>
       </c>
-      <c r="K16" s="49" t="s">
+      <c r="K16" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="50"/>
-    </row>
-    <row r="17" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="55"/>
+    </row>
+    <row r="17" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>13</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>733</v>
+        <v>590</v>
       </c>
       <c r="C17" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1556,50 +1756,50 @@
         <f ca="1">IF(C17 = 0.6, G16, 0)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>308</v>
-      </c>
-      <c r="G17" s="35"/>
+        <v>164</v>
+      </c>
+      <c r="G17" s="34"/>
       <c r="I17" s="17" t="s">
         <v>17</v>
       </c>
       <c r="J17" s="21">
         <v>0.18</v>
       </c>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="48"/>
-    </row>
-    <row r="18" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
+      <c r="L17" s="53"/>
+    </row>
+    <row r="18" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57">
         <v>14</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>308</v>
+        <v>164</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <f ca="1">IF(C17 = 0.4, G16, 0)</f>
-        <v>931</v>
-      </c>
-      <c r="E18" s="30">
+        <v>901</v>
+      </c>
+      <c r="E18" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>764</v>
-      </c>
-      <c r="G18" s="35">
+        <v>604</v>
+      </c>
+      <c r="G18" s="34">
         <f ca="1">IF(F18 &lt; J29, (IF(F18&lt;0, J28, J28-F18)), 0 )</f>
-        <v>900</v>
+        <v>887</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>19</v>
@@ -1608,61 +1808,61 @@
         <f>J16*J17</f>
         <v>17.37</v>
       </c>
-      <c r="K18" s="49" t="s">
+      <c r="K18" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="48"/>
-    </row>
-    <row r="19" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="53"/>
+    </row>
+    <row r="19" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>15</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>764</v>
+        <v>604</v>
       </c>
       <c r="C19" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D19" s="1">
         <f ca="1">IF(C19 = 0.6, G18, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="30">
+        <v>887</v>
+      </c>
+      <c r="E19" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>459</v>
+        <v>371</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>305</v>
-      </c>
-      <c r="G19" s="35"/>
-    </row>
-    <row r="20" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
+        <v>1120</v>
+      </c>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57">
         <v>16</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>305</v>
+        <v>1120</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <f ca="1">IF(C19 = 0.4, G18, 0)</f>
-        <v>900</v>
-      </c>
-      <c r="E20" s="30">
+        <v>0</v>
+      </c>
+      <c r="E20" s="29">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J6, K6))</f>
-        <v>447</v>
+        <v>485</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>758</v>
-      </c>
-      <c r="G20" s="35">
-        <f ca="1">IF(F20 &lt; J29, (IF(F20&lt;0, J28, J28-F20)), 0 )</f>
-        <v>906</v>
+        <v>635</v>
+      </c>
+      <c r="G20" s="34">
+        <f ca="1">IF(F20 &lt; M29, (IF(F20&lt;0, M28, M28-F20)), 0 )</f>
+        <v>1332</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>13</v>
@@ -1676,31 +1876,31 @@
       <c r="L20" s="18"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>17</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>758</v>
+        <v>635</v>
       </c>
       <c r="C21" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D21" s="1">
         <f ca="1">IF(C21 = 0.6, G20, 0)</f>
-        <v>906</v>
-      </c>
-      <c r="E21" s="31">
+        <v>0</v>
+      </c>
+      <c r="E21" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>527</v>
+        <v>616</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1137</v>
-      </c>
-      <c r="G21" s="35"/>
+        <v>19</v>
+      </c>
+      <c r="G21" s="34"/>
       <c r="I21" s="20" t="s">
         <v>21</v>
       </c>
@@ -1708,48 +1908,48 @@
         <f>20+2*J20</f>
         <v>34</v>
       </c>
-      <c r="K21" s="44" t="s">
+      <c r="K21" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="45"/>
-    </row>
-    <row r="22" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="L21" s="50"/>
+    </row>
+    <row r="22" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="57">
         <v>18</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1137</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <f ca="1">IF(C21 = 0.4, G20, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="31">
+        <v>1332</v>
+      </c>
+      <c r="E22" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>589</v>
+        <v>530</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>548</v>
-      </c>
-      <c r="G22" s="35">
-        <f ca="1">IF(F22 &lt; J29, (IF(F22&lt;0, J28, J28-F22)), 0 )</f>
-        <v>1116</v>
+        <v>821</v>
+      </c>
+      <c r="G22" s="34">
+        <f ca="1">IF(F22 &lt; M29, (IF(F22&lt;0, M28, M28-F22)), 0 )</f>
+        <v>1146</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-    </row>
-    <row r="23" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+    </row>
+    <row r="23" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>19</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>548</v>
+        <v>821</v>
       </c>
       <c r="C23" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1759,189 +1959,215 @@
         <f ca="1">IF(C23 = 0.6, G22, 0)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>509</v>
+        <v>570</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="G23" s="35"/>
+        <v>251</v>
+      </c>
+      <c r="G23" s="34"/>
       <c r="I23" s="17" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="21">
         <v>900</v>
       </c>
-      <c r="K23" s="44" t="s">
+      <c r="K23" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="L23" s="45"/>
+      <c r="L23" s="50"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
+    <row r="24" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57">
         <v>20</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>251</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <f ca="1">IF(C23 = 0.4, G22, 0)</f>
-        <v>1116</v>
-      </c>
-      <c r="E24" s="31">
+        <v>1146</v>
+      </c>
+      <c r="E24" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>511</v>
+        <v>580</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>644</v>
-      </c>
-      <c r="G24" s="35">
-        <f ca="1">IF(F24 &lt; J29, (IF(F24&lt;0, J28, J28-F24)), 0 )</f>
-        <v>1020</v>
+        <v>817</v>
+      </c>
+      <c r="G24" s="34">
+        <f ca="1">IF(F24 &lt; M29, (IF(F24&lt;0, M28, M28-F24)), 0 )</f>
+        <v>1150</v>
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>21</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>644</v>
+        <v>817</v>
       </c>
       <c r="C25" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D25" s="1">
         <f ca="1">IF(C25 = 0.6, G24, 0)</f>
-        <v>1020</v>
-      </c>
-      <c r="E25" s="31">
+        <v>0</v>
+      </c>
+      <c r="E25" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>443</v>
+        <v>507</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1221</v>
-      </c>
-      <c r="G25" s="35"/>
+        <v>310</v>
+      </c>
+      <c r="G25" s="34"/>
       <c r="I25" s="20" t="s">
         <v>25</v>
       </c>
       <c r="J25" s="21">
         <v>2</v>
       </c>
-      <c r="K25" s="44" t="s">
+      <c r="K25" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="45"/>
-    </row>
-    <row r="26" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
+      <c r="L25" s="50"/>
+    </row>
+    <row r="26" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="57">
         <v>22</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1221</v>
+        <v>310</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
         <f ca="1">IF(C25 = 0.4, G24, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="31">
+        <v>1150</v>
+      </c>
+      <c r="E26" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>566</v>
+        <v>674</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>655</v>
-      </c>
-      <c r="G26" s="35">
-        <f ca="1">IF(F26 &lt; J29, (IF(F26&lt;0, J28, J28-F26)), 0 )</f>
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+        <v>786</v>
+      </c>
+      <c r="G26" s="34">
+        <f ca="1">IF(F26 &lt; M29, (IF(F26&lt;0, M28, M28-F26)), 0 )</f>
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="27">
         <v>23</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>655</v>
+        <v>786</v>
       </c>
       <c r="C27" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D27" s="1">
         <f ca="1">IF(C27 = 0.6, G26, 0)</f>
-        <v>1009</v>
-      </c>
-      <c r="E27" s="31">
+        <v>0</v>
+      </c>
+      <c r="E27" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
         <v>528</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1136</v>
-      </c>
-      <c r="G27" s="35"/>
-      <c r="I27" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="J27" s="47"/>
-    </row>
-    <row r="28" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A28" s="27">
+        <v>258</v>
+      </c>
+      <c r="G27" s="34"/>
+      <c r="I27" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="52"/>
+      <c r="L27" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="M27" s="68"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="P27" s="68"/>
+      <c r="Q27" s="62"/>
+    </row>
+    <row r="28" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A28" s="57">
         <v>24</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1136</v>
+        <v>258</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
         <f ca="1">IF(C27 = 0.4, G26, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="31">
+        <v>1181</v>
+      </c>
+      <c r="E28" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>585</v>
+        <v>607</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>551</v>
-      </c>
-      <c r="G28" s="35">
-        <f ca="1">IF(F28 &lt; J29, (IF(F28&lt;0, J28, J28-F28)), 0 )</f>
-        <v>1113</v>
+        <v>832</v>
+      </c>
+      <c r="G28" s="34">
+        <f ca="1">IF(F28 &lt; M29, (IF(F28&lt;0, M28, M28-F28)), 0 )</f>
+        <v>1135</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J28" s="22">
-        <f>INT(J41+N39*J42)</f>
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <f>INT(M33 + M34*M37)</f>
+        <v>1491</v>
+      </c>
+      <c r="L28" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="64">
+        <f>INT(O33 + O34*O37)</f>
+        <v>1967</v>
+      </c>
+      <c r="N28" s="62"/>
+      <c r="O28" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="P28" s="64">
+        <f>INT(Q33 + Q34*Q37)</f>
+        <v>1193</v>
+      </c>
+      <c r="Q28" s="62"/>
+    </row>
+    <row r="29" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
         <v>25</v>
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>551</v>
+        <v>832</v>
       </c>
       <c r="C29" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -1949,116 +2175,132 @@
       </c>
       <c r="D29" s="1">
         <f ca="1">IF(C29 = 0.6, G28, 0)</f>
-        <v>1113</v>
-      </c>
-      <c r="E29" s="31">
+        <v>1135</v>
+      </c>
+      <c r="E29" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>454</v>
+        <v>567</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1210</v>
-      </c>
-      <c r="G29" s="35"/>
+        <v>1400</v>
+      </c>
+      <c r="G29" s="34"/>
       <c r="I29" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J29" s="23">
         <f>IF(INT(J28-207.456) &lt; 0, 0, INT(J28-207.456) )</f>
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27">
+        <v>1283</v>
+      </c>
+      <c r="L29" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" s="66">
+        <f>IF(INT(M28-207.456) &lt; 0, 0, INT(M28-207.456) )</f>
+        <v>1759</v>
+      </c>
+      <c r="N29" s="62"/>
+      <c r="O29" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" s="66">
+        <f>IF(INT(P28-207.456) &lt; 0, 0, INT(P28-207.456) )</f>
+        <v>985</v>
+      </c>
+      <c r="Q29" s="62"/>
+    </row>
+    <row r="30" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="57">
         <v>26</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1210</v>
+        <v>1400</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <f ca="1">IF(C29 = 0.4, G28, 0)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="31">
+      <c r="E30" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>577</v>
+        <v>635</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>633</v>
-      </c>
-      <c r="G30" s="35">
-        <f ca="1">IF(F30 &lt; J29, (IF(F30&lt;0, J28, J28-F30)), 0 )</f>
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>765</v>
+      </c>
+      <c r="G30" s="34">
+        <f ca="1">IF(F30 &lt; M29, (IF(F30&lt;0, M28, M28-F30)), 0 )</f>
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <v>27</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>633</v>
+        <v>765</v>
       </c>
       <c r="C31" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D31" s="1">
         <f ca="1">IF(C31 = 0.6, G30, 0)</f>
-        <v>1031</v>
-      </c>
-      <c r="E31" s="31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>507</v>
+        <v>549</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1157</v>
-      </c>
-      <c r="G31" s="35"/>
-      <c r="I31" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="G31" s="34"/>
+      <c r="I31" s="36" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27">
+      <c r="J31" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="57">
         <v>28</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1157</v>
+        <v>216</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
         <f ca="1">IF(C31 = 0.4, G30, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="31">
+        <v>1202</v>
+      </c>
+      <c r="E32" s="30">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J7, K7))</f>
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>578</v>
-      </c>
-      <c r="G32" s="35">
-        <f ca="1">IF(F32 &lt; J29, (IF(F32&lt;0, J28, J28-F32)), 0 )</f>
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>849</v>
+      </c>
+      <c r="G32" s="34">
+        <f ca="1">IF(F32 &lt; P29, (IF(F32&lt;0, P28, P28-F32)), 0 )</f>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
         <v>29</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>578</v>
+        <v>849</v>
       </c>
       <c r="C33" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2068,56 +2310,98 @@
         <f ca="1">IF(C33 = 0.6, G32, 0)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>367</v>
+        <v>331</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>211</v>
-      </c>
-      <c r="G33" s="35"/>
-      <c r="I33" s="52" t="s">
-        <v>35</v>
+        <v>518</v>
+      </c>
+      <c r="G33" s="34"/>
+      <c r="I33" s="43" t="s">
+        <v>34</v>
       </c>
       <c r="J33" s="21">
-        <f>INT(J28-J29+(N5*2/2))</f>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="27">
+        <f ca="1">INT(AVERAGE(B5:B54))</f>
+        <v>542</v>
+      </c>
+      <c r="L33" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" s="21">
+        <f>INT(J6*(J25+((I11*J11) + (I12*J12))))</f>
+        <v>1479</v>
+      </c>
+      <c r="N33" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="O33" s="71">
+        <f>INT(J7*(J25+((I11*J11) + (I12*J12))))</f>
+        <v>1955</v>
+      </c>
+      <c r="P33" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q33" s="71">
+        <f>INT(J8*(J25+((I11*J11) + (I12*J12))))</f>
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="57">
         <v>30</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>211</v>
+        <v>518</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
         <f ca="1">IF(C33 = 0.4, G32, 0)</f>
-        <v>1086</v>
-      </c>
-      <c r="E34" s="32">
+        <v>344</v>
+      </c>
+      <c r="E34" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>329</v>
+        <v>420</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>968</v>
-      </c>
-      <c r="G34" s="35">
-        <f ca="1">IF(F34 &lt; J29, (IF(F34&lt;0, J28, J28-F34)), 0 )</f>
-        <v>696</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+      <c r="G34" s="34">
+        <f ca="1">IF(F34 &lt; P29, (IF(F34&lt;0, P28, P28-F34)), 0 )</f>
+        <v>751</v>
+      </c>
+      <c r="L34" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="M34" s="21">
+        <f>INT(SQRT((J25+((I11*J11)+(I12*J12)))*K6))</f>
+        <v>11</v>
+      </c>
+      <c r="N34" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="O34" s="71">
+        <f>INT(SQRT((J25+((I11*J11)+(I12*J12)))*K7))</f>
+        <v>13</v>
+      </c>
+      <c r="P34" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q34" s="71">
+        <f>INT(SQRT((J25+((I11*J11)+(I12*J12)))*K8))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <v>31</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>968</v>
+        <v>442</v>
       </c>
       <c r="C35" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2127,253 +2411,292 @@
         <f ca="1">IF(C35 = 0.6, G34, 0)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>627</v>
-      </c>
-      <c r="G35" s="35"/>
-      <c r="I35" s="52" t="s">
-        <v>37</v>
+        <v>115</v>
+      </c>
+      <c r="G35" s="34"/>
+      <c r="I35" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="J35" s="21">
         <f ca="1">COUNTIF(F5:F54,"&lt;0")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="57">
         <v>32</v>
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>627</v>
+        <v>115</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
         <f ca="1">IF(C35 = 0.4, G34, 0)</f>
-        <v>696</v>
-      </c>
-      <c r="E36" s="32">
+        <v>751</v>
+      </c>
+      <c r="E36" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>336</v>
+        <v>266</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>987</v>
-      </c>
-      <c r="G36" s="35">
-        <f ca="1">IF(F36 &lt; J29, (IF(F36&lt;0, J28, J28-F36)), 0 )</f>
-        <v>677</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+      <c r="G36" s="34">
+        <f ca="1">IF(F36 &lt; P29, (IF(F36&lt;0, P28, P28-F36)), 0 )</f>
+        <v>593</v>
+      </c>
+      <c r="L36" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="M36" s="73">
+        <f>1/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="N36" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="O36" s="73">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P36" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q36" s="73">
+        <f>1/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
         <v>33</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>987</v>
+        <v>600</v>
       </c>
       <c r="C37" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D37" s="1">
         <f ca="1">IF(C37 = 0.6, G36, 0)</f>
-        <v>677</v>
-      </c>
-      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="E37" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1343</v>
-      </c>
-      <c r="G37" s="35"/>
-      <c r="I37" s="52" t="s">
-        <v>38</v>
+        <v>310</v>
+      </c>
+      <c r="G37" s="34"/>
+      <c r="I37" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="J37" s="21">
         <f>(J18*(J25/50)/J21)</f>
         <v>2.0435294117647062E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
+      <c r="L37" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="M37" s="73">
+        <f>ABS(NORMSINV(M36))</f>
+        <v>1.1503493803760083</v>
+      </c>
+      <c r="N37" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="O37" s="73">
+        <f>ABS(NORMSINV(O36))</f>
+        <v>0.96742156610170071</v>
+      </c>
+      <c r="P37" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q37" s="74">
+        <f>ABS(NORMSINV(Q36))</f>
+        <v>1.3351777361189361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="57">
         <v>34</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1343</v>
+        <v>310</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
         <f ca="1">IF(C37 = 0.4, G36, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="32">
+        <v>593</v>
+      </c>
+      <c r="E38" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>998</v>
-      </c>
-      <c r="G38" s="35">
-        <f ca="1">IF(F38 &lt; J29, (IF(F38&lt;0, J28, J28-F38)), 0 )</f>
-        <v>666</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="G38" s="34">
+        <f ca="1">IF(F38 &lt; P29, (IF(F38&lt;0, P28, P28-F38)), 0 )</f>
+        <v>634</v>
+      </c>
+      <c r="K38" s="59"/>
+      <c r="L38" s="59"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="59"/>
+    </row>
+    <row r="39" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
         <v>35</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>998</v>
+        <v>559</v>
       </c>
       <c r="C39" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D39" s="1">
         <f ca="1">IF(C39 = 0.6, G38, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="32">
+        <v>634</v>
+      </c>
+      <c r="E39" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>659</v>
-      </c>
-      <c r="G39" s="35"/>
-      <c r="I39" s="52" t="s">
-        <v>39</v>
+        <v>852</v>
+      </c>
+      <c r="G39" s="34"/>
+      <c r="I39" s="43" t="s">
+        <v>38</v>
       </c>
       <c r="J39" s="21">
-        <f>1/(50/2)</f>
+        <f ca="1">1/(COUNTIF(G5:G54,"&gt;0"))</f>
         <v>0.04</v>
       </c>
-      <c r="K39" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="L39" s="21">
-        <v>58</v>
-      </c>
-      <c r="M39" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="N39" s="54">
-        <f>(3*L39)/100</f>
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="27">
+      <c r="K39" s="60"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="60"/>
+      <c r="N39" s="61"/>
+    </row>
+    <row r="40" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A40" s="57">
         <v>36</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>659</v>
+        <v>852</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1">
         <f ca="1">IF(C39 = 0.4, G38, 0)</f>
-        <v>666</v>
-      </c>
-      <c r="E40" s="32">
+        <v>0</v>
+      </c>
+      <c r="E40" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>977</v>
-      </c>
-      <c r="G40" s="35">
-        <f ca="1">IF(F40 &lt; J29, (IF(F40&lt;0, J28, J28-F40)), 0 )</f>
-        <v>687</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+      <c r="G40" s="34">
+        <f ca="1">IF(F40 &lt; P29, (IF(F40&lt;0, P28, P28-F40)), 0 )</f>
+        <v>700</v>
+      </c>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+    </row>
+    <row r="41" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" s="27">
         <v>37</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>977</v>
+        <v>493</v>
       </c>
       <c r="C41" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D41" s="1">
         <f ca="1">IF(C41 = 0.6, G40, 0)</f>
-        <v>687</v>
-      </c>
-      <c r="E41" s="32">
+        <v>0</v>
+      </c>
+      <c r="E41" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>282</v>
+        <v>379</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1382</v>
-      </c>
-      <c r="G41" s="35"/>
-      <c r="I41" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="J41" s="21">
-        <f>N5*(2+(0.6*1 + 0.4*2))</f>
-        <v>1538.6133333333332</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
+        <v>114</v>
+      </c>
+      <c r="G41" s="34"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="59"/>
+      <c r="L41" s="59"/>
+      <c r="M41" s="59"/>
+      <c r="N41" s="59"/>
+    </row>
+    <row r="42" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A42" s="57">
         <v>38</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1382</v>
+        <v>114</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1">
         <f ca="1">IF(C41 = 0.4, G40, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="32">
+        <v>700</v>
+      </c>
+      <c r="E42" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>411</v>
+        <v>321</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>971</v>
-      </c>
-      <c r="G42" s="35">
-        <f ca="1">IF(F42 &lt; J29, (IF(F42&lt;0, J28, J28-F42)), 0 )</f>
-        <v>693</v>
-      </c>
-      <c r="I42" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="J42" s="56">
-        <f>SQRT((N6^2)*(2+ (1*0.6 + 2*0.4)))</f>
-        <v>72.595430620280766</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+      <c r="G42" s="34">
+        <f ca="1">IF(F42 &lt; P29, (IF(F42&lt;0, P28, P28-F42)), 0 )</f>
+        <v>700</v>
+      </c>
+      <c r="I42" s="60"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+    </row>
+    <row r="43" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <v>39</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>971</v>
+        <v>493</v>
       </c>
       <c r="C43" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2383,55 +2706,56 @@
         <f ca="1">IF(C43 = 0.6, G42, 0)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="32">
+      <c r="E43" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>617</v>
-      </c>
-      <c r="G43" s="35"/>
-    </row>
-    <row r="44" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="27">
+        <v>127</v>
+      </c>
+      <c r="G43" s="34"/>
+    </row>
+    <row r="44" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="57">
         <v>40</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>617</v>
+        <v>127</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1">
         <f ca="1">IF(C43 = 0.4, G42, 0)</f>
-        <v>693</v>
-      </c>
-      <c r="E44" s="32">
+        <v>700</v>
+      </c>
+      <c r="E44" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>364</v>
+        <v>301</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>946</v>
-      </c>
-      <c r="G44" s="35">
-        <f ca="1">IF(F44 &lt; J29, (IF(F44&lt;0, J28, J28-F44)), 0 )</f>
-        <v>718</v>
-      </c>
-      <c r="I44" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="J44" s="55">
-        <v>1.4501999999999999E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+        <v>526</v>
+      </c>
+      <c r="G44" s="34">
+        <f ca="1">IF(F44 &lt; P29, (IF(F44&lt;0, P28, P28-F44)), 0 )</f>
+        <v>667</v>
+      </c>
+      <c r="I44" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="J44" s="45">
+        <f ca="1">ABS(SUMIF(F5:F54,"&lt;0"))/ COUNTIF(G5:G54,"&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A45" s="27">
         <v>41</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>946</v>
+        <v>526</v>
       </c>
       <c r="C45" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2439,101 +2763,101 @@
       </c>
       <c r="D45" s="1">
         <f ca="1">IF(C45 = 0.6, G44, 0)</f>
-        <v>718</v>
-      </c>
-      <c r="E45" s="32">
+        <v>667</v>
+      </c>
+      <c r="E45" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1332</v>
-      </c>
-      <c r="G45" s="35"/>
-    </row>
-    <row r="46" spans="1:14" ht="19" x14ac:dyDescent="0.2">
-      <c r="A46" s="27">
+        <v>871</v>
+      </c>
+      <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A46" s="57">
         <v>42</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1332</v>
+        <v>871</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1">
         <f ca="1">IF(C45 = 0.4, G44, 0)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="32">
+      <c r="E46" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>392</v>
+        <v>345</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>940</v>
-      </c>
-      <c r="G46" s="35">
-        <f ca="1">IF(F46 &lt; J29, (IF(F46&lt;0, J28, J28-F46)), 0 )</f>
-        <v>724</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="G46" s="34">
+        <f ca="1">IF(F46 &lt; P29, (IF(F46&lt;0, P28, P28-F46)), 0 )</f>
+        <v>667</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
         <v>43</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>940</v>
+        <v>526</v>
       </c>
       <c r="C47" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D47" s="1">
         <f ca="1">IF(C47 = 0.6, G46, 0)</f>
-        <v>724</v>
-      </c>
-      <c r="E47" s="32">
+        <v>0</v>
+      </c>
+      <c r="E47" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>321</v>
+        <v>401</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1343</v>
-      </c>
-      <c r="G47" s="35"/>
-    </row>
-    <row r="48" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="27">
+        <v>125</v>
+      </c>
+      <c r="G47" s="34"/>
+    </row>
+    <row r="48" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="57">
         <v>44</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1343</v>
+        <v>125</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
         <f ca="1">IF(C47 = 0.4, G46, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="32">
+        <v>667</v>
+      </c>
+      <c r="E48" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>305</v>
+        <v>365</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1038</v>
-      </c>
-      <c r="G48" s="35">
-        <f ca="1">IF(F48 &lt; J29, (IF(F48&lt;0, J28, J28-F48)), 0 )</f>
-        <v>626</v>
-      </c>
-      <c r="I48" s="52" t="s">
-        <v>46</v>
+        <v>427</v>
+      </c>
+      <c r="G48" s="34">
+        <f ca="1">IF(F48 &lt; P29, (IF(F48&lt;0, P28, P28-F48)), 0 )</f>
+        <v>766</v>
+      </c>
+      <c r="I48" s="43" t="s">
+        <v>41</v>
       </c>
       <c r="J48" s="21">
-        <f>(J18*J33)+(J21*J44/2)+(J23/2)</f>
-        <v>11914.446534000001</v>
+        <f ca="1">(J18*J33)+(J21*J35)+(J23*COUNTIF(G5:G54,"&gt;0"))</f>
+        <v>31914.54</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2542,7 +2866,7 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1038</v>
+        <v>427</v>
       </c>
       <c r="C49" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2552,40 +2876,40 @@
         <f ca="1">IF(C49 = 0.6, G48, 0)</f>
         <v>0</v>
       </c>
-      <c r="E49" s="32">
+      <c r="E49" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>282</v>
+        <v>309</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>756</v>
-      </c>
-      <c r="G49" s="35"/>
+        <v>118</v>
+      </c>
+      <c r="G49" s="34"/>
     </row>
     <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A50" s="27">
+      <c r="A50" s="57">
         <v>46</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>756</v>
+        <v>118</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1">
         <f ca="1">IF(C49 = 0.4, G48, 0)</f>
-        <v>626</v>
-      </c>
-      <c r="E50" s="32">
+        <v>766</v>
+      </c>
+      <c r="E50" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>388</v>
+        <v>355</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>994</v>
-      </c>
-      <c r="G50" s="35">
-        <f ca="1">IF(F50 &lt; J29, (IF(F50&lt;0, J28, J28-F50)), 0 )</f>
-        <v>670</v>
+        <v>529</v>
+      </c>
+      <c r="G50" s="34">
+        <f ca="1">IF(F50 &lt; P29, (IF(F50&lt;0, P28, P28-F50)), 0 )</f>
+        <v>664</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2594,7 +2918,7 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>994</v>
+        <v>529</v>
       </c>
       <c r="C51" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2604,40 +2928,40 @@
         <f ca="1">IF(C51 = 0.6, G50, 0)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="32">
+      <c r="E51" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>652</v>
-      </c>
-      <c r="G51" s="35"/>
+        <v>195</v>
+      </c>
+      <c r="G51" s="34"/>
     </row>
     <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A52" s="27">
+      <c r="A52" s="57">
         <v>48</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>652</v>
+        <v>195</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1">
         <f ca="1">IF(C51 = 0.4, G50, 0)</f>
-        <v>670</v>
-      </c>
-      <c r="E52" s="32">
+        <v>664</v>
+      </c>
+      <c r="E52" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>287</v>
+        <v>370</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1035</v>
-      </c>
-      <c r="G52" s="35">
-        <f ca="1">IF(F52 &lt; J29, (IF(F52&lt;0, J28, J28-F52)), 0 )</f>
-        <v>629</v>
+        <v>489</v>
+      </c>
+      <c r="G52" s="34">
+        <f ca="1">IF(F52 &lt; P29, (IF(F52&lt;0, P28, P28-F52)), 0 )</f>
+        <v>704</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2646,7 +2970,7 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1035</v>
+        <v>489</v>
       </c>
       <c r="C53" s="1">
         <f ca="1">PROB(I11:I12,J11:J12,RANDBETWEEN(1,2))</f>
@@ -2656,181 +2980,182 @@
         <f ca="1">IF(C53 = 0.6, G52, 0)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="32">
+      <c r="E53" s="31">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>414</v>
+        <v>386</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>621</v>
-      </c>
-      <c r="G53" s="35"/>
+        <v>103</v>
+      </c>
+      <c r="G53" s="34"/>
     </row>
     <row r="54" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="28">
+      <c r="A54" s="58">
         <v>50</v>
       </c>
-      <c r="B54" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>621</v>
+      <c r="B54" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>103</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
         <f ca="1">IF(C53 = 0.4, G52, 0)</f>
-        <v>629</v>
-      </c>
-      <c r="E54" s="33">
+        <v>704</v>
+      </c>
+      <c r="E54" s="32">
         <f ca="1">INT(_xlfn.NORM.INV(RAND(), J8, K8))</f>
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>883</v>
-      </c>
-      <c r="G54" s="36">
-        <f ca="1">IF(F54 &lt; J29, (IF(F54&lt;0, J28, J28-F54)), 0 )</f>
-        <v>781</v>
+        <v>505</v>
+      </c>
+      <c r="G54" s="35">
+        <f ca="1">IF(F54 &lt; P29, (IF(F54&lt;0, P28, P28-F54)), 0 )</f>
+        <v>688</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B59" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C59" s="43" t="s">
+      <c r="A59" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" s="42" t="s">
         <v>28</v>
       </c>
+      <c r="C59" s="42" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="40">
+      <c r="A60" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="41">
+      <c r="A61" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="41">
+      <c r="A62" s="40">
         <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="41">
+      <c r="A63" s="40">
         <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="41">
+      <c r="A64" s="40">
         <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="41">
+      <c r="A65" s="40">
         <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="41">
+      <c r="A66" s="40">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="41">
+      <c r="A67" s="40">
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="41">
+      <c r="A68" s="40">
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="41">
+      <c r="A69" s="40">
         <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="41">
+      <c r="A70" s="40">
         <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="41">
+      <c r="A71" s="40">
         <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="41">
+      <c r="A72" s="40">
         <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="41">
+      <c r="A73" s="40">
         <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="41">
+      <c r="A74" s="40">
         <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="41">
+      <c r="A75" s="40">
         <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="41">
+      <c r="A76" s="40">
         <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="41">
+      <c r="A77" s="40">
         <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="41">
+      <c r="A78" s="40">
         <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="41">
+      <c r="A79" s="40">
         <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="41">
+      <c r="A80" s="40">
         <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="41">
+      <c r="A81" s="40">
         <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="41">
+      <c r="A82" s="40">
         <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="41">
+      <c r="A83" s="40">
         <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="42">
+      <c r="A84" s="41">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="O27:P27"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="K17:L17"/>
@@ -2839,6 +3164,7 @@
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K23:L23"/>
+    <mergeCell ref="L27:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>